<commit_message>
Calculate updated ratios for meoh process from latest ANL data
</commit_message>
<xml_diff>
--- a/use_cases/LWR_MeOH_2023/data/HERON_data.xlsx
+++ b/use_cases/LWR_MeOH_2023/data/HERON_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWR_MeOH_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D16D78-4ADD-1949-B922-E27C21077EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4689BC62-852B-A848-96A1-302D3FD5988E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="2" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sweep values" sheetId="10" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Capacity_Market" sheetId="3" r:id="rId6"/>
     <sheet name="NPP_capacities" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="188">
   <si>
     <t>Source</t>
   </si>
@@ -508,15 +508,9 @@
     <t xml:space="preserve">naphtha </t>
   </si>
   <si>
-    <t>Inputs (MT/y)</t>
-  </si>
-  <si>
     <t xml:space="preserve">co2 </t>
   </si>
   <si>
-    <t>Fuel products (MMgal/y)</t>
-  </si>
-  <si>
     <t>jet fuel</t>
   </si>
   <si>
@@ -541,9 +535,6 @@
     <t>Inputs (kg/h)</t>
   </si>
   <si>
-    <t>Fuel products (gal/h)</t>
-  </si>
-  <si>
     <t>Fuel products (kg/h)</t>
   </si>
   <si>
@@ -602,15 +593,28 @@
   </si>
   <si>
     <t>SA sweep values</t>
+  </si>
+  <si>
+    <t>Inputs (MT/d)</t>
+  </si>
+  <si>
+    <t>Fuel products (MT/d)</t>
+  </si>
+  <si>
+    <t>electricity (MW)</t>
+  </si>
+  <si>
+    <t>Ratios\Scale(MWe)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -659,7 +663,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -688,8 +692,14 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -881,6 +891,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -889,7 +938,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -917,13 +966,38 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="12" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="16" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -936,37 +1010,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="5" borderId="12" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="5" borderId="16" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -1043,7 +1107,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>MeOH!$D$36</c:f>
+              <c:f>MeOH!$D$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1120,7 +1184,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>MeOH!$C$37:$C$39</c:f>
+              <c:f>MeOH!$C$34:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1138,7 +1202,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MeOH!$D$37:$D$39</c:f>
+              <c:f>MeOH!$D$34:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1999,16 +2063,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2335,7 +2399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
@@ -2478,52 +2542,52 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>178</v>
-      </c>
-      <c r="B15" s="33">
+        <v>175</v>
+      </c>
+      <c r="B15" s="28">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B16">
-        <f>MeOH!B47</f>
-        <v>22.260273972602739</v>
+        <f>MeOH!B44</f>
+        <v>24.166666666666664</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="D18" s="56"/>
-      <c r="E18" s="55" t="s">
-        <v>183</v>
-      </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="55" t="s">
+      <c r="D18" s="46"/>
+      <c r="E18" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" s="46"/>
+      <c r="G18" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="56"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="41"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="54"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="11" t="s">
         <v>74</v>
       </c>
@@ -2553,34 +2617,34 @@
       <c r="A20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B20">
         <v>1194</v>
       </c>
-      <c r="C20" s="50">
+      <c r="C20">
         <f>MAX(-B20+$B$15, -1000+$B$15)</f>
         <v>-1000</v>
       </c>
-      <c r="D20" s="50">
+      <c r="D20">
         <f>-100+$B$15</f>
         <v>-100</v>
       </c>
-      <c r="E20" s="51">
+      <c r="E20" s="39">
         <f>C20*$B$16</f>
-        <v>-22260.273972602739</v>
-      </c>
-      <c r="F20" s="51">
+        <v>-24166.666666666664</v>
+      </c>
+      <c r="F20" s="39">
         <f>D20*$B$16</f>
-        <v>-2226.027397260274</v>
-      </c>
-      <c r="G20" s="43">
+        <v>-2416.6666666666665</v>
+      </c>
+      <c r="G20" s="34">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H20" s="43">
+      <c r="H20" s="34">
         <f>ABS(E20)*24*I20</f>
-        <v>1068493.1506849315</v>
-      </c>
-      <c r="I20" s="50">
+        <v>1160000</v>
+      </c>
+      <c r="I20">
         <f t="shared" ref="I20:I22" si="0">ROUNDUP(J20*$I$24/$J$24,0)</f>
         <v>2</v>
       </c>
@@ -2592,34 +2656,34 @@
       <c r="A21" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B21" s="50">
+      <c r="B21">
         <v>769</v>
       </c>
-      <c r="C21" s="50">
+      <c r="C21">
         <f t="shared" ref="C21:C24" si="1">MAX(-B21+$B$15, -1000+$B$15)</f>
         <v>-769</v>
       </c>
-      <c r="D21" s="50">
+      <c r="D21">
         <f t="shared" ref="D21:D24" si="2">-100+$B$15</f>
         <v>-100</v>
       </c>
-      <c r="E21" s="51">
+      <c r="E21" s="39">
         <f t="shared" ref="E21:E24" si="3">C21*$B$16</f>
-        <v>-17118.150684931508</v>
-      </c>
-      <c r="F21" s="51">
+        <v>-18584.166666666664</v>
+      </c>
+      <c r="F21" s="39">
         <f t="shared" ref="F21:F24" si="4">D21*$B$16</f>
-        <v>-2226.027397260274</v>
-      </c>
-      <c r="G21" s="43">
+        <v>-2416.6666666666665</v>
+      </c>
+      <c r="G21" s="34">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H21" s="43">
+      <c r="H21" s="34">
         <f t="shared" ref="H21:H23" si="5">ABS(E21)*24*I21</f>
-        <v>2875849.3150684936</v>
-      </c>
-      <c r="I21" s="50">
+        <v>3122139.9999999995</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -2631,34 +2695,34 @@
       <c r="A22" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="50">
+      <c r="B22">
         <v>894</v>
       </c>
-      <c r="C22" s="50">
+      <c r="C22">
         <f t="shared" si="1"/>
         <v>-894</v>
       </c>
-      <c r="D22" s="50">
+      <c r="D22">
         <f t="shared" si="2"/>
         <v>-100</v>
       </c>
-      <c r="E22" s="51">
+      <c r="E22" s="39">
         <f t="shared" si="3"/>
-        <v>-19900.68493150685</v>
-      </c>
-      <c r="F22" s="51">
+        <v>-21604.999999999996</v>
+      </c>
+      <c r="F22" s="39">
         <f t="shared" si="4"/>
-        <v>-2226.027397260274</v>
-      </c>
-      <c r="G22" s="43">
+        <v>-2416.6666666666665</v>
+      </c>
+      <c r="G22" s="34">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H22" s="43">
+      <c r="H22" s="34">
         <f t="shared" si="5"/>
-        <v>955232.87671232875</v>
-      </c>
-      <c r="I22" s="50">
+        <v>1037039.9999999998</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2670,34 +2734,34 @@
       <c r="A23" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="50">
+      <c r="B23">
         <v>522</v>
       </c>
-      <c r="C23" s="50">
+      <c r="C23">
         <f t="shared" si="1"/>
         <v>-522</v>
       </c>
-      <c r="D23" s="50">
+      <c r="D23">
         <f t="shared" si="2"/>
         <v>-100</v>
       </c>
-      <c r="E23" s="51">
+      <c r="E23" s="39">
         <f t="shared" si="3"/>
-        <v>-11619.86301369863</v>
-      </c>
-      <c r="F23" s="51">
+        <v>-12614.999999999998</v>
+      </c>
+      <c r="F23" s="39">
         <f t="shared" si="4"/>
-        <v>-2226.027397260274</v>
-      </c>
-      <c r="G23" s="43">
+        <v>-2416.6666666666665</v>
+      </c>
+      <c r="G23" s="34">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H23" s="43">
+      <c r="H23" s="34">
         <f t="shared" si="5"/>
-        <v>278876.71232876711</v>
-      </c>
-      <c r="I23" s="50">
+        <v>302759.99999999994</v>
+      </c>
+      <c r="I23">
         <f>ROUNDUP(J23*$I$24/$J$24,0)</f>
         <v>1</v>
       </c>
@@ -2720,21 +2784,21 @@
         <f t="shared" si="2"/>
         <v>-100</v>
       </c>
-      <c r="E24" s="52">
+      <c r="E24" s="40">
         <f t="shared" si="3"/>
-        <v>-22260.273972602739</v>
-      </c>
-      <c r="F24" s="52">
+        <v>-24166.666666666664</v>
+      </c>
+      <c r="F24" s="40">
         <f t="shared" si="4"/>
-        <v>-2226.027397260274</v>
-      </c>
-      <c r="G24" s="46">
+        <v>-2416.6666666666665</v>
+      </c>
+      <c r="G24" s="37">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H24" s="46">
+      <c r="H24" s="37">
         <f>ABS(E24)*24*I24</f>
-        <v>7479452.0547945211</v>
+        <v>8120000</v>
       </c>
       <c r="I24" s="19">
         <v>14</v>
@@ -2752,37 +2816,37 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="40">
+      <c r="B27" s="31">
         <v>0</v>
       </c>
-      <c r="C27" s="40">
+      <c r="C27" s="31">
         <v>1</v>
       </c>
-      <c r="D27" s="40">
+      <c r="D27" s="31">
         <v>2</v>
       </c>
-      <c r="E27" s="40">
+      <c r="E27" s="31">
         <v>3</v>
       </c>
-      <c r="F27" s="40">
+      <c r="F27" s="31">
         <v>4</v>
       </c>
-      <c r="G27" s="40">
+      <c r="G27" s="31">
         <v>5</v>
       </c>
-      <c r="H27" s="40">
+      <c r="H27" s="31">
         <v>6</v>
       </c>
-      <c r="I27" s="40">
+      <c r="I27" s="31">
         <v>7</v>
       </c>
-      <c r="J27" s="40">
+      <c r="J27" s="31">
         <v>8</v>
       </c>
-      <c r="K27" s="41">
+      <c r="K27" s="32">
         <v>9</v>
       </c>
     </row>
@@ -2790,43 +2854,43 @@
       <c r="A28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="42">
+      <c r="B28" s="33">
         <f>$C20+B$27*ABS($C20-$D20)/9</f>
         <v>-1000</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="34">
         <f t="shared" ref="C28:K28" si="6">$C20+C$27*ABS($C20-$D20)/9</f>
         <v>-900</v>
       </c>
-      <c r="D28" s="42">
+      <c r="D28" s="33">
         <f t="shared" si="6"/>
         <v>-800</v>
       </c>
-      <c r="E28" s="43">
+      <c r="E28" s="34">
         <f t="shared" si="6"/>
         <v>-700</v>
       </c>
-      <c r="F28" s="42">
+      <c r="F28" s="33">
         <f t="shared" si="6"/>
         <v>-600</v>
       </c>
-      <c r="G28" s="43">
+      <c r="G28" s="34">
         <f t="shared" si="6"/>
         <v>-500</v>
       </c>
-      <c r="H28" s="42">
+      <c r="H28" s="33">
         <f t="shared" si="6"/>
         <v>-400</v>
       </c>
-      <c r="I28" s="43">
+      <c r="I28" s="34">
         <f t="shared" si="6"/>
         <v>-300</v>
       </c>
-      <c r="J28" s="42">
+      <c r="J28" s="33">
         <f t="shared" si="6"/>
         <v>-200</v>
       </c>
-      <c r="K28" s="44">
+      <c r="K28" s="35">
         <f t="shared" si="6"/>
         <v>-100</v>
       </c>
@@ -2835,43 +2899,43 @@
       <c r="A29" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="42">
+      <c r="B29" s="33">
         <f t="shared" ref="B29:K32" si="7">$C21+B$27*ABS($C21-$D21)/9</f>
         <v>-769</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="34">
         <f t="shared" si="7"/>
         <v>-694.66666666666663</v>
       </c>
-      <c r="D29" s="42">
+      <c r="D29" s="33">
         <f t="shared" si="7"/>
         <v>-620.33333333333337</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="34">
         <f t="shared" si="7"/>
         <v>-546</v>
       </c>
-      <c r="F29" s="42">
+      <c r="F29" s="33">
         <f t="shared" si="7"/>
         <v>-471.66666666666669</v>
       </c>
-      <c r="G29" s="43">
+      <c r="G29" s="34">
         <f t="shared" si="7"/>
         <v>-397.33333333333331</v>
       </c>
-      <c r="H29" s="42">
+      <c r="H29" s="33">
         <f t="shared" si="7"/>
         <v>-323</v>
       </c>
-      <c r="I29" s="43">
+      <c r="I29" s="34">
         <f t="shared" si="7"/>
         <v>-248.66666666666663</v>
       </c>
-      <c r="J29" s="42">
+      <c r="J29" s="33">
         <f t="shared" si="7"/>
         <v>-174.33333333333337</v>
       </c>
-      <c r="K29" s="44">
+      <c r="K29" s="35">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
@@ -2880,43 +2944,43 @@
       <c r="A30" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="42">
+      <c r="B30" s="33">
         <f t="shared" si="7"/>
         <v>-894</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="34">
         <f t="shared" si="7"/>
         <v>-805.77777777777783</v>
       </c>
-      <c r="D30" s="42">
+      <c r="D30" s="33">
         <f t="shared" si="7"/>
         <v>-717.55555555555554</v>
       </c>
-      <c r="E30" s="43">
+      <c r="E30" s="34">
         <f t="shared" si="7"/>
         <v>-629.33333333333326</v>
       </c>
-      <c r="F30" s="42">
+      <c r="F30" s="33">
         <f t="shared" si="7"/>
         <v>-541.11111111111109</v>
       </c>
-      <c r="G30" s="43">
+      <c r="G30" s="34">
         <f t="shared" si="7"/>
         <v>-452.88888888888891</v>
       </c>
-      <c r="H30" s="42">
+      <c r="H30" s="33">
         <f t="shared" si="7"/>
         <v>-364.66666666666663</v>
       </c>
-      <c r="I30" s="43">
+      <c r="I30" s="34">
         <f t="shared" si="7"/>
         <v>-276.44444444444446</v>
       </c>
-      <c r="J30" s="42">
+      <c r="J30" s="33">
         <f t="shared" si="7"/>
         <v>-188.22222222222217</v>
       </c>
-      <c r="K30" s="44">
+      <c r="K30" s="35">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
@@ -2925,43 +2989,43 @@
       <c r="A31" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B31" s="42">
+      <c r="B31" s="33">
         <f t="shared" si="7"/>
         <v>-522</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="34">
         <f t="shared" si="7"/>
         <v>-475.11111111111109</v>
       </c>
-      <c r="D31" s="42">
+      <c r="D31" s="33">
         <f t="shared" si="7"/>
         <v>-428.22222222222223</v>
       </c>
-      <c r="E31" s="43">
+      <c r="E31" s="34">
         <f t="shared" si="7"/>
         <v>-381.33333333333337</v>
       </c>
-      <c r="F31" s="42">
+      <c r="F31" s="33">
         <f t="shared" si="7"/>
         <v>-334.44444444444446</v>
       </c>
-      <c r="G31" s="43">
+      <c r="G31" s="34">
         <f t="shared" si="7"/>
         <v>-287.55555555555554</v>
       </c>
-      <c r="H31" s="42">
+      <c r="H31" s="33">
         <f t="shared" si="7"/>
         <v>-240.66666666666669</v>
       </c>
-      <c r="I31" s="43">
+      <c r="I31" s="34">
         <f t="shared" si="7"/>
         <v>-193.77777777777777</v>
       </c>
-      <c r="J31" s="42">
+      <c r="J31" s="33">
         <f t="shared" si="7"/>
         <v>-146.88888888888891</v>
       </c>
-      <c r="K31" s="44">
+      <c r="K31" s="35">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
@@ -2970,84 +3034,84 @@
       <c r="A32" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="45">
+      <c r="B32" s="36">
         <f t="shared" si="7"/>
         <v>-1000</v>
       </c>
-      <c r="C32" s="46">
+      <c r="C32" s="37">
         <f t="shared" si="7"/>
         <v>-900</v>
       </c>
-      <c r="D32" s="45">
+      <c r="D32" s="36">
         <f t="shared" si="7"/>
         <v>-800</v>
       </c>
-      <c r="E32" s="46">
+      <c r="E32" s="37">
         <f t="shared" si="7"/>
         <v>-700</v>
       </c>
-      <c r="F32" s="45">
+      <c r="F32" s="36">
         <f t="shared" si="7"/>
         <v>-600</v>
       </c>
-      <c r="G32" s="46">
+      <c r="G32" s="37">
         <f t="shared" si="7"/>
         <v>-500</v>
       </c>
-      <c r="H32" s="45">
+      <c r="H32" s="36">
         <f t="shared" si="7"/>
         <v>-400</v>
       </c>
-      <c r="I32" s="46">
+      <c r="I32" s="37">
         <f t="shared" si="7"/>
         <v>-300</v>
       </c>
-      <c r="J32" s="45">
+      <c r="J32" s="36">
         <f t="shared" si="7"/>
         <v>-200</v>
       </c>
-      <c r="K32" s="47">
+      <c r="K32" s="38">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="40">
+      <c r="B35" s="31">
         <v>0</v>
       </c>
-      <c r="C35" s="40">
+      <c r="C35" s="31">
         <v>1</v>
       </c>
-      <c r="D35" s="40">
+      <c r="D35" s="31">
         <v>2</v>
       </c>
-      <c r="E35" s="40">
+      <c r="E35" s="31">
         <v>3</v>
       </c>
-      <c r="F35" s="40">
+      <c r="F35" s="31">
         <v>4</v>
       </c>
-      <c r="G35" s="40">
+      <c r="G35" s="31">
         <v>5</v>
       </c>
-      <c r="H35" s="40">
+      <c r="H35" s="31">
         <v>6</v>
       </c>
-      <c r="I35" s="40">
+      <c r="I35" s="31">
         <v>7</v>
       </c>
-      <c r="J35" s="40">
+      <c r="J35" s="31">
         <v>8</v>
       </c>
-      <c r="K35" s="41">
+      <c r="K35" s="32">
         <v>9</v>
       </c>
     </row>
@@ -3055,225 +3119,225 @@
       <c r="A36" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="42">
+      <c r="B36" s="33">
         <f>$E20+B$35*ABS($E20-$F20)/9</f>
-        <v>-22260.273972602739</v>
-      </c>
-      <c r="C36" s="43">
+        <v>-24166.666666666664</v>
+      </c>
+      <c r="C36" s="34">
         <f t="shared" ref="C36:K36" si="8">$E20+C$35*ABS($E20-$F20)/9</f>
-        <v>-20034.246575342466</v>
-      </c>
-      <c r="D36" s="42">
+        <v>-21750</v>
+      </c>
+      <c r="D36" s="33">
         <f t="shared" si="8"/>
-        <v>-17808.219178082192</v>
-      </c>
-      <c r="E36" s="43">
+        <v>-19333.333333333332</v>
+      </c>
+      <c r="E36" s="34">
         <f t="shared" si="8"/>
-        <v>-15582.191780821917</v>
-      </c>
-      <c r="F36" s="42">
+        <v>-16916.666666666664</v>
+      </c>
+      <c r="F36" s="33">
         <f t="shared" si="8"/>
-        <v>-13356.164383561643</v>
-      </c>
-      <c r="G36" s="43">
+        <v>-14500</v>
+      </c>
+      <c r="G36" s="34">
         <f t="shared" si="8"/>
-        <v>-11130.13698630137</v>
-      </c>
-      <c r="H36" s="42">
+        <v>-12083.333333333332</v>
+      </c>
+      <c r="H36" s="33">
         <f t="shared" si="8"/>
-        <v>-8904.1095890410943</v>
-      </c>
-      <c r="I36" s="43">
+        <v>-9666.6666666666679</v>
+      </c>
+      <c r="I36" s="34">
         <f t="shared" si="8"/>
-        <v>-6678.0821917808207</v>
-      </c>
-      <c r="J36" s="42">
+        <v>-7250</v>
+      </c>
+      <c r="J36" s="33">
         <f t="shared" si="8"/>
-        <v>-4452.0547945205471</v>
-      </c>
-      <c r="K36" s="44">
+        <v>-4833.3333333333358</v>
+      </c>
+      <c r="K36" s="35">
         <f t="shared" si="8"/>
-        <v>-2226.0273972602736</v>
+        <v>-2416.6666666666679</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B37" s="42">
+      <c r="B37" s="33">
         <f t="shared" ref="B37:K40" si="9">$E21+B$35*ABS($E21-$F21)/9</f>
-        <v>-17118.150684931508</v>
-      </c>
-      <c r="C37" s="43">
+        <v>-18584.166666666664</v>
+      </c>
+      <c r="C37" s="34">
         <f t="shared" si="9"/>
-        <v>-15463.470319634704</v>
-      </c>
-      <c r="D37" s="42">
+        <v>-16787.777777777774</v>
+      </c>
+      <c r="D37" s="33">
         <f t="shared" si="9"/>
-        <v>-13808.789954337901</v>
-      </c>
-      <c r="E37" s="43">
+        <v>-14991.388888888887</v>
+      </c>
+      <c r="E37" s="34">
         <f t="shared" si="9"/>
-        <v>-12154.109589041096</v>
-      </c>
-      <c r="F37" s="42">
+        <v>-13194.999999999998</v>
+      </c>
+      <c r="F37" s="33">
         <f t="shared" si="9"/>
-        <v>-10499.429223744293</v>
-      </c>
-      <c r="G37" s="43">
+        <v>-11398.611111111109</v>
+      </c>
+      <c r="G37" s="34">
         <f t="shared" si="9"/>
-        <v>-8844.7488584474886</v>
-      </c>
-      <c r="H37" s="42">
+        <v>-9602.2222222222208</v>
+      </c>
+      <c r="H37" s="33">
         <f t="shared" si="9"/>
-        <v>-7190.0684931506839</v>
-      </c>
-      <c r="I37" s="43">
+        <v>-7805.8333333333321</v>
+      </c>
+      <c r="I37" s="34">
         <f t="shared" si="9"/>
-        <v>-5535.3881278538811</v>
-      </c>
-      <c r="J37" s="42">
+        <v>-6009.4444444444434</v>
+      </c>
+      <c r="J37" s="33">
         <f t="shared" si="9"/>
-        <v>-3880.7077625570782</v>
-      </c>
-      <c r="K37" s="44">
+        <v>-4213.0555555555547</v>
+      </c>
+      <c r="K37" s="35">
         <f t="shared" si="9"/>
-        <v>-2226.0273972602718</v>
+        <v>-2416.6666666666679</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="42">
+      <c r="B38" s="33">
         <f t="shared" si="9"/>
-        <v>-19900.68493150685</v>
-      </c>
-      <c r="C38" s="43">
+        <v>-21604.999999999996</v>
+      </c>
+      <c r="C38" s="34">
         <f t="shared" si="9"/>
-        <v>-17936.834094368343</v>
-      </c>
-      <c r="D38" s="42">
+        <v>-19472.96296296296</v>
+      </c>
+      <c r="D38" s="33">
         <f t="shared" si="9"/>
-        <v>-15972.983257229833</v>
-      </c>
-      <c r="E38" s="43">
+        <v>-17340.925925925923</v>
+      </c>
+      <c r="E38" s="34">
         <f t="shared" si="9"/>
-        <v>-14009.132420091326</v>
-      </c>
-      <c r="F38" s="42">
+        <v>-15208.888888888887</v>
+      </c>
+      <c r="F38" s="33">
         <f t="shared" si="9"/>
-        <v>-12045.281582952815</v>
-      </c>
-      <c r="G38" s="43">
+        <v>-13076.85185185185</v>
+      </c>
+      <c r="G38" s="34">
         <f t="shared" si="9"/>
-        <v>-10081.430745814307</v>
-      </c>
-      <c r="H38" s="42">
+        <v>-10944.814814814814</v>
+      </c>
+      <c r="H38" s="33">
         <f t="shared" si="9"/>
-        <v>-8117.5799086757997</v>
-      </c>
-      <c r="I38" s="43">
+        <v>-8812.7777777777774</v>
+      </c>
+      <c r="I38" s="34">
         <f t="shared" si="9"/>
-        <v>-6153.729071537291</v>
-      </c>
-      <c r="J38" s="42">
+        <v>-6680.7407407407391</v>
+      </c>
+      <c r="J38" s="33">
         <f t="shared" si="9"/>
-        <v>-4189.8782343987823</v>
-      </c>
-      <c r="K38" s="44">
+        <v>-4548.7037037037044</v>
+      </c>
+      <c r="K38" s="35">
         <f t="shared" si="9"/>
-        <v>-2226.0273972602736</v>
+        <v>-2416.6666666666679</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="42">
+      <c r="B39" s="33">
         <f t="shared" si="9"/>
-        <v>-11619.86301369863</v>
-      </c>
-      <c r="C39" s="43">
+        <v>-12614.999999999998</v>
+      </c>
+      <c r="C39" s="34">
         <f t="shared" si="9"/>
-        <v>-10576.103500761035</v>
-      </c>
-      <c r="D39" s="42">
+        <v>-11481.85185185185</v>
+      </c>
+      <c r="D39" s="33">
         <f t="shared" si="9"/>
-        <v>-9532.3439878234403</v>
-      </c>
-      <c r="E39" s="43">
+        <v>-10348.703703703703</v>
+      </c>
+      <c r="E39" s="34">
         <f t="shared" si="9"/>
-        <v>-8488.5844748858453</v>
-      </c>
-      <c r="F39" s="42">
+        <v>-9215.5555555555547</v>
+      </c>
+      <c r="F39" s="33">
         <f t="shared" si="9"/>
-        <v>-7444.8249619482494</v>
-      </c>
-      <c r="G39" s="43">
+        <v>-8082.407407407406</v>
+      </c>
+      <c r="G39" s="34">
         <f t="shared" si="9"/>
-        <v>-6401.0654490106544</v>
-      </c>
-      <c r="H39" s="42">
+        <v>-6949.2592592592582</v>
+      </c>
+      <c r="H39" s="33">
         <f t="shared" si="9"/>
-        <v>-5357.3059360730595</v>
-      </c>
-      <c r="I39" s="43">
+        <v>-5816.1111111111104</v>
+      </c>
+      <c r="I39" s="34">
         <f t="shared" si="9"/>
-        <v>-4313.5464231354645</v>
-      </c>
-      <c r="J39" s="42">
+        <v>-4682.9629629629617</v>
+      </c>
+      <c r="J39" s="33">
         <f t="shared" si="9"/>
-        <v>-3269.7869101978686</v>
-      </c>
-      <c r="K39" s="44">
+        <v>-3549.8148148148139</v>
+      </c>
+      <c r="K39" s="35">
         <f t="shared" si="9"/>
-        <v>-2226.0273972602736</v>
+        <v>-2416.6666666666661</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B40" s="45">
+      <c r="B40" s="36">
         <f t="shared" si="9"/>
-        <v>-22260.273972602739</v>
-      </c>
-      <c r="C40" s="46">
+        <v>-24166.666666666664</v>
+      </c>
+      <c r="C40" s="37">
         <f t="shared" si="9"/>
-        <v>-20034.246575342466</v>
-      </c>
-      <c r="D40" s="45">
+        <v>-21750</v>
+      </c>
+      <c r="D40" s="36">
         <f t="shared" si="9"/>
-        <v>-17808.219178082192</v>
-      </c>
-      <c r="E40" s="46">
+        <v>-19333.333333333332</v>
+      </c>
+      <c r="E40" s="37">
         <f t="shared" si="9"/>
-        <v>-15582.191780821917</v>
-      </c>
-      <c r="F40" s="45">
+        <v>-16916.666666666664</v>
+      </c>
+      <c r="F40" s="36">
         <f t="shared" si="9"/>
-        <v>-13356.164383561643</v>
-      </c>
-      <c r="G40" s="46">
+        <v>-14500</v>
+      </c>
+      <c r="G40" s="37">
         <f t="shared" si="9"/>
-        <v>-11130.13698630137</v>
-      </c>
-      <c r="H40" s="45">
+        <v>-12083.333333333332</v>
+      </c>
+      <c r="H40" s="36">
         <f t="shared" si="9"/>
-        <v>-8904.1095890410943</v>
-      </c>
-      <c r="I40" s="46">
+        <v>-9666.6666666666679</v>
+      </c>
+      <c r="I40" s="37">
         <f t="shared" si="9"/>
-        <v>-6678.0821917808207</v>
-      </c>
-      <c r="J40" s="45">
+        <v>-7250</v>
+      </c>
+      <c r="J40" s="36">
         <f t="shared" si="9"/>
-        <v>-4452.0547945205471</v>
-      </c>
-      <c r="K40" s="47">
+        <v>-4833.3333333333358</v>
+      </c>
+      <c r="K40" s="38">
         <f t="shared" si="9"/>
-        <v>-2226.0273972602736</v>
+        <v>-2416.6666666666679</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3282,37 +3346,37 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="40">
+      <c r="B43" s="31">
         <v>0</v>
       </c>
-      <c r="C43" s="40">
+      <c r="C43" s="31">
         <v>1</v>
       </c>
-      <c r="D43" s="40">
+      <c r="D43" s="31">
         <v>2</v>
       </c>
-      <c r="E43" s="40">
+      <c r="E43" s="31">
         <v>3</v>
       </c>
-      <c r="F43" s="40">
+      <c r="F43" s="31">
         <v>4</v>
       </c>
-      <c r="G43" s="40">
+      <c r="G43" s="31">
         <v>5</v>
       </c>
-      <c r="H43" s="40">
+      <c r="H43" s="31">
         <v>6</v>
       </c>
-      <c r="I43" s="40">
+      <c r="I43" s="31">
         <v>7</v>
       </c>
-      <c r="J43" s="40">
+      <c r="J43" s="31">
         <v>8</v>
       </c>
-      <c r="K43" s="41">
+      <c r="K43" s="32">
         <v>9</v>
       </c>
     </row>
@@ -3320,230 +3384,230 @@
       <c r="A44" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B44" s="42">
+      <c r="B44" s="33">
         <f>B$43*ABS($G20-$H20)/9</f>
         <v>0</v>
       </c>
-      <c r="C44" s="43">
+      <c r="C44" s="34">
         <f t="shared" ref="C44:J44" si="10">C$43*ABS($G20-$H20)/9</f>
-        <v>118721.46118721462</v>
-      </c>
-      <c r="D44" s="42">
+        <v>128888.88888888889</v>
+      </c>
+      <c r="D44" s="33">
         <f t="shared" si="10"/>
-        <v>237442.92237442924</v>
-      </c>
-      <c r="E44" s="43">
+        <v>257777.77777777778</v>
+      </c>
+      <c r="E44" s="34">
         <f t="shared" si="10"/>
-        <v>356164.38356164389</v>
-      </c>
-      <c r="F44" s="42">
+        <v>386666.66666666669</v>
+      </c>
+      <c r="F44" s="33">
         <f t="shared" si="10"/>
-        <v>474885.84474885848</v>
-      </c>
-      <c r="G44" s="43">
+        <v>515555.55555555556</v>
+      </c>
+      <c r="G44" s="34">
         <f t="shared" si="10"/>
-        <v>593607.30593607307</v>
-      </c>
-      <c r="H44" s="42">
+        <v>644444.4444444445</v>
+      </c>
+      <c r="H44" s="33">
         <f t="shared" si="10"/>
-        <v>712328.76712328778</v>
-      </c>
-      <c r="I44" s="43">
+        <v>773333.33333333337</v>
+      </c>
+      <c r="I44" s="34">
         <f t="shared" si="10"/>
-        <v>831050.22831050237</v>
-      </c>
-      <c r="J44" s="42">
+        <v>902222.22222222225</v>
+      </c>
+      <c r="J44" s="33">
         <f t="shared" si="10"/>
-        <v>949771.68949771696</v>
-      </c>
-      <c r="K44" s="44">
+        <v>1031111.1111111111</v>
+      </c>
+      <c r="K44" s="35">
         <f>K$43*ABS($G20-$H20)/9</f>
-        <v>1068493.1506849315</v>
+        <v>1160000</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B45" s="42">
+      <c r="B45" s="33">
         <f t="shared" ref="B45:K45" si="11">B$43*ABS($G21-$H21)/9</f>
         <v>0</v>
       </c>
-      <c r="C45" s="43">
+      <c r="C45" s="34">
         <f t="shared" si="11"/>
-        <v>319538.8127853882</v>
-      </c>
-      <c r="D45" s="42">
+        <v>346904.44444444438</v>
+      </c>
+      <c r="D45" s="33">
         <f t="shared" si="11"/>
-        <v>639077.62557077641</v>
-      </c>
-      <c r="E45" s="43">
+        <v>693808.88888888876</v>
+      </c>
+      <c r="E45" s="34">
         <f t="shared" si="11"/>
-        <v>958616.43835616438</v>
-      </c>
-      <c r="F45" s="42">
+        <v>1040713.3333333331</v>
+      </c>
+      <c r="F45" s="33">
         <f t="shared" si="11"/>
-        <v>1278155.2511415528</v>
-      </c>
-      <c r="G45" s="43">
+        <v>1387617.7777777775</v>
+      </c>
+      <c r="G45" s="34">
         <f t="shared" si="11"/>
-        <v>1597694.063926941</v>
-      </c>
-      <c r="H45" s="42">
+        <v>1734522.222222222</v>
+      </c>
+      <c r="H45" s="33">
         <f t="shared" si="11"/>
-        <v>1917232.8767123288</v>
-      </c>
-      <c r="I45" s="43">
+        <v>2081426.6666666663</v>
+      </c>
+      <c r="I45" s="34">
         <f t="shared" si="11"/>
-        <v>2236771.6894977172</v>
-      </c>
-      <c r="J45" s="42">
+        <v>2428331.1111111105</v>
+      </c>
+      <c r="J45" s="33">
         <f t="shared" si="11"/>
-        <v>2556310.5022831056</v>
-      </c>
-      <c r="K45" s="44">
+        <v>2775235.555555555</v>
+      </c>
+      <c r="K45" s="35">
         <f t="shared" si="11"/>
-        <v>2875849.3150684936</v>
+        <v>3122139.9999999995</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="42">
+      <c r="B46" s="33">
         <f t="shared" ref="B46:K46" si="12">B$43*ABS($G22-$H22)/9</f>
         <v>0</v>
       </c>
-      <c r="C46" s="43">
+      <c r="C46" s="34">
         <f t="shared" si="12"/>
-        <v>106136.98630136986</v>
-      </c>
-      <c r="D46" s="42">
+        <v>115226.66666666664</v>
+      </c>
+      <c r="D46" s="33">
         <f t="shared" si="12"/>
-        <v>212273.97260273973</v>
-      </c>
-      <c r="E46" s="43">
+        <v>230453.33333333328</v>
+      </c>
+      <c r="E46" s="34">
         <f t="shared" si="12"/>
-        <v>318410.9589041096</v>
-      </c>
-      <c r="F46" s="42">
+        <v>345679.99999999988</v>
+      </c>
+      <c r="F46" s="33">
         <f t="shared" si="12"/>
-        <v>424547.94520547945</v>
-      </c>
-      <c r="G46" s="43">
+        <v>460906.66666666657</v>
+      </c>
+      <c r="G46" s="34">
         <f t="shared" si="12"/>
-        <v>530684.93150684936</v>
-      </c>
-      <c r="H46" s="42">
+        <v>576133.33333333326</v>
+      </c>
+      <c r="H46" s="33">
         <f t="shared" si="12"/>
-        <v>636821.91780821921</v>
-      </c>
-      <c r="I46" s="43">
+        <v>691359.99999999977</v>
+      </c>
+      <c r="I46" s="34">
         <f t="shared" si="12"/>
-        <v>742958.90410958906</v>
-      </c>
-      <c r="J46" s="42">
+        <v>806586.66666666651</v>
+      </c>
+      <c r="J46" s="33">
         <f t="shared" si="12"/>
-        <v>849095.89041095891</v>
-      </c>
-      <c r="K46" s="44">
+        <v>921813.33333333314</v>
+      </c>
+      <c r="K46" s="35">
         <f t="shared" si="12"/>
-        <v>955232.87671232887</v>
+        <v>1037039.9999999998</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B47" s="42">
+      <c r="B47" s="33">
         <f t="shared" ref="B47:K47" si="13">B$43*ABS($G23-$H23)/9</f>
         <v>0</v>
       </c>
-      <c r="C47" s="43">
+      <c r="C47" s="34">
         <f t="shared" si="13"/>
-        <v>30986.301369863013</v>
-      </c>
-      <c r="D47" s="42">
+        <v>33639.999999999993</v>
+      </c>
+      <c r="D47" s="33">
         <f t="shared" si="13"/>
-        <v>61972.602739726026</v>
-      </c>
-      <c r="E47" s="43">
+        <v>67279.999999999985</v>
+      </c>
+      <c r="E47" s="34">
         <f t="shared" si="13"/>
-        <v>92958.904109589028</v>
-      </c>
-      <c r="F47" s="42">
+        <v>100919.99999999997</v>
+      </c>
+      <c r="F47" s="33">
         <f t="shared" si="13"/>
-        <v>123945.20547945205</v>
-      </c>
-      <c r="G47" s="43">
+        <v>134559.99999999997</v>
+      </c>
+      <c r="G47" s="34">
         <f t="shared" si="13"/>
-        <v>154931.50684931508</v>
-      </c>
-      <c r="H47" s="42">
+        <v>168199.99999999997</v>
+      </c>
+      <c r="H47" s="33">
         <f t="shared" si="13"/>
-        <v>185917.80821917806</v>
-      </c>
-      <c r="I47" s="43">
+        <v>201839.99999999994</v>
+      </c>
+      <c r="I47" s="34">
         <f t="shared" si="13"/>
-        <v>216904.10958904109</v>
-      </c>
-      <c r="J47" s="42">
+        <v>235479.99999999994</v>
+      </c>
+      <c r="J47" s="33">
         <f t="shared" si="13"/>
-        <v>247890.4109589041</v>
-      </c>
-      <c r="K47" s="44">
+        <v>269119.99999999994</v>
+      </c>
+      <c r="K47" s="35">
         <f t="shared" si="13"/>
-        <v>278876.71232876711</v>
+        <v>302759.99999999994</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B48" s="45">
+      <c r="B48" s="36">
         <f t="shared" ref="B48:K48" si="14">B$43*ABS($G24-$H24)/9</f>
         <v>0</v>
       </c>
-      <c r="C48" s="46">
+      <c r="C48" s="37">
         <f t="shared" si="14"/>
-        <v>831050.22831050237</v>
-      </c>
-      <c r="D48" s="45">
+        <v>902222.22222222225</v>
+      </c>
+      <c r="D48" s="36">
         <f t="shared" si="14"/>
-        <v>1662100.4566210047</v>
-      </c>
-      <c r="E48" s="46">
+        <v>1804444.4444444445</v>
+      </c>
+      <c r="E48" s="37">
         <f t="shared" si="14"/>
-        <v>2493150.6849315073</v>
-      </c>
-      <c r="F48" s="45">
+        <v>2706666.6666666665</v>
+      </c>
+      <c r="F48" s="36">
         <f t="shared" si="14"/>
-        <v>3324200.9132420095</v>
-      </c>
-      <c r="G48" s="46">
+        <v>3608888.888888889</v>
+      </c>
+      <c r="G48" s="37">
         <f t="shared" si="14"/>
-        <v>4155251.1415525121</v>
-      </c>
-      <c r="H48" s="45">
+        <v>4511111.111111111</v>
+      </c>
+      <c r="H48" s="36">
         <f t="shared" si="14"/>
-        <v>4986301.3698630147</v>
-      </c>
-      <c r="I48" s="46">
+        <v>5413333.333333333</v>
+      </c>
+      <c r="I48" s="37">
         <f t="shared" si="14"/>
-        <v>5817351.5981735168</v>
-      </c>
-      <c r="J48" s="45">
+        <v>6315555.555555556</v>
+      </c>
+      <c r="J48" s="36">
         <f t="shared" si="14"/>
-        <v>6648401.8264840189</v>
-      </c>
-      <c r="K48" s="47">
+        <v>7217777.777777778</v>
+      </c>
+      <c r="K48" s="38">
         <f t="shared" si="14"/>
-        <v>7479452.054794522</v>
+        <v>8120000</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="38" t="s">
-        <v>186</v>
+      <c r="A51" s="29" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -3584,10 +3648,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="47"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -3717,10 +3781,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E49A404-39E7-6B45-B584-7FD70EB84AF5}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3728,25 +3792,26 @@
     <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2">
         <v>1.2E-2</v>
       </c>
       <c r="G2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H2">
         <v>3.7854100000000002</v>
@@ -3754,7 +3819,7 @@
     </row>
     <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3771,7 +3836,7 @@
         <v>1000</v>
       </c>
       <c r="G4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H4">
         <v>0.77</v>
@@ -3794,7 +3859,7 @@
         <v>655027563.25600004</v>
       </c>
       <c r="G5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H5">
         <v>0.8</v>
@@ -3817,7 +3882,7 @@
         <v>27050057.672000002</v>
       </c>
       <c r="G6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H6">
         <v>0.85</v>
@@ -3829,7 +3894,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B8">
         <f>SUM(B9:B13)</f>
@@ -3922,23 +3987,23 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>142</v>
       </c>
@@ -3952,337 +4017,390 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>165</v>
-      </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+    <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="F20" s="67" t="s">
+        <v>187</v>
+      </c>
+      <c r="G20" s="20">
+        <v>100</v>
+      </c>
+      <c r="H20" s="20">
+        <v>500</v>
+      </c>
+      <c r="I20" s="21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="B21" s="29">
-        <f>MeOH_original_data!B18*1000/(365*24)</f>
-        <v>2226.027397260274</v>
-      </c>
-      <c r="C21" s="29">
-        <f>MeOH_original_data!C18*1000/(365*24)</f>
-        <v>11130.13698630137</v>
-      </c>
-      <c r="D21" s="30">
-        <f>MeOH_original_data!D18*1000/(365*24)</f>
-        <v>22260.273972602739</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="B21" s="58">
+        <f>MeOH_original_data!B18*1000/(24)</f>
+        <v>2416.6666666666665</v>
+      </c>
+      <c r="C21" s="58">
+        <f>MeOH_original_data!C18*1000/(24)</f>
+        <v>12125</v>
+      </c>
+      <c r="D21" s="59">
+        <f>MeOH_original_data!D18*1000/(24)</f>
+        <v>24291.666666666668</v>
+      </c>
+      <c r="F21" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="G21" s="63">
+        <v>1</v>
+      </c>
+      <c r="H21" s="63">
+        <v>1</v>
+      </c>
+      <c r="I21" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" s="60">
+        <f>MeOH_original_data!B19*1000/(24)</f>
+        <v>14666.666666666666</v>
+      </c>
+      <c r="C22" s="60">
+        <f>MeOH_original_data!C19*1000/(24)</f>
+        <v>73375</v>
+      </c>
+      <c r="D22" s="61">
+        <f>MeOH_original_data!D19*1000/(24)</f>
+        <v>146791.66666666666</v>
+      </c>
+      <c r="F22" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="G22" s="63">
+        <f>G$21*B22/B$21</f>
+        <v>6.068965517241379</v>
+      </c>
+      <c r="H22" s="63">
+        <f t="shared" ref="H22:I26" si="1">H$21*C22/C21</f>
+        <v>6.0515463917525771</v>
+      </c>
+      <c r="I22" s="64">
+        <f>I$21*D22/D21</f>
+        <v>6.0428816466552311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B23" s="62">
+        <f>MeOH_original_data!B20</f>
+        <v>5.5</v>
+      </c>
+      <c r="C23" s="62">
+        <f>MeOH_original_data!C20</f>
+        <v>27</v>
+      </c>
+      <c r="D23" s="62">
+        <f>MeOH_original_data!D20</f>
+        <v>53</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>146</v>
+      </c>
+      <c r="G23" s="63">
+        <f t="shared" ref="G23:G26" si="2">G$21*B23/B$21</f>
+        <v>2.2758620689655173E-3</v>
+      </c>
+      <c r="H23" s="63">
+        <f t="shared" si="1"/>
+        <v>3.6797274275979556E-4</v>
+      </c>
+      <c r="I23" s="64">
+        <f t="shared" si="1"/>
+        <v>3.6105591825149024E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="46"/>
+      <c r="F24" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" s="63">
+        <f>G$21*B25/B$21</f>
+        <v>4.1379310344827586E-2</v>
+      </c>
+      <c r="H24" s="63">
+        <f t="shared" ref="H24:I24" si="3">H$21*C25/C$21</f>
+        <v>4.192439862542955E-2</v>
+      </c>
+      <c r="I24" s="64">
+        <f t="shared" si="3"/>
+        <v>4.1852487135506003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" s="52">
+        <f>MeOH_original_data!B22*1000/(24)</f>
+        <v>100</v>
+      </c>
+      <c r="C25" s="52">
+        <f>MeOH_original_data!C22*1000/(24)</f>
+        <v>508.33333333333331</v>
+      </c>
+      <c r="D25" s="53">
+        <f>MeOH_original_data!D22*1000/(24)</f>
+        <v>1016.6666666666666</v>
+      </c>
+      <c r="F25" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="B22" s="29">
-        <f>MeOH_original_data!B19*1000/(365*24)</f>
-        <v>13384.817351598174</v>
-      </c>
-      <c r="C22" s="29">
-        <f>MeOH_original_data!C19*1000/(365*24)</f>
-        <v>66917.922374429225</v>
-      </c>
-      <c r="D22" s="30">
-        <f>MeOH_original_data!D19*1000/(365*24)</f>
-        <v>133848.74429223745</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="37"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="B24" s="27">
-        <f>MeOH_original_data!B21*1000000/(365*24)</f>
-        <v>70.776255707762559</v>
-      </c>
-      <c r="C24" s="27">
-        <f>MeOH_original_data!C21*1000000/(365*24)</f>
-        <v>352.73972602739724</v>
-      </c>
-      <c r="D24" s="28">
-        <f>MeOH_original_data!D21*1000000/(365*24)</f>
-        <v>705.47945205479448</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B25" s="27">
-        <f>MeOH_original_data!B22*1000000/(365*24)</f>
-        <v>303.65296803652967</v>
-      </c>
-      <c r="C25" s="27">
-        <f>MeOH_original_data!C22*1000000/(365*24)</f>
-        <v>1519.4063926940639</v>
-      </c>
-      <c r="D25" s="28">
-        <f>MeOH_original_data!D22*1000000/(365*24)</f>
-        <v>3039.9543378995436</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="63">
+        <f t="shared" ref="G25:G26" si="4">G$21*B26/B$21</f>
+        <v>0.34655172413793106</v>
+      </c>
+      <c r="H25" s="63">
+        <f t="shared" ref="H25:H26" si="5">H$21*C26/C$21</f>
+        <v>0.3446735395189004</v>
+      </c>
+      <c r="I25" s="64">
+        <f t="shared" ref="I25:I26" si="6">I$21*D26/D$21</f>
+        <v>0.34425385934819897</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B26" s="27">
-        <f>MeOH_original_data!B23*1000000/(365*24)</f>
-        <v>1114.1552511415525</v>
-      </c>
-      <c r="C26" s="27">
-        <f>MeOH_original_data!C23*1000000/(365*24)</f>
-        <v>5567.3515981735163</v>
-      </c>
-      <c r="D26" s="28">
-        <f>MeOH_original_data!D23*1000000/(365*24)</f>
-        <v>11135.844748858448</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="str">
-        <f>A24</f>
-        <v xml:space="preserve">naphtha </v>
-      </c>
-      <c r="B28" s="29">
-        <f>B24*$H$2*$H4</f>
-        <v>206.29620251141554</v>
-      </c>
-      <c r="C28" s="29">
-        <f t="shared" ref="C28:D28" si="1">C24*$H$2*$H4</f>
-        <v>1028.1536544520548</v>
-      </c>
-      <c r="D28" s="30">
-        <f t="shared" si="1"/>
-        <v>2056.3073089041095</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="str">
-        <f t="shared" ref="A29:A30" si="2">A25</f>
-        <v>jet fuel</v>
-      </c>
-      <c r="B29" s="29">
-        <f t="shared" ref="B29:D29" si="3">B25*$H$2*$H5</f>
-        <v>919.5607853881279</v>
-      </c>
-      <c r="C29" s="29">
-        <f t="shared" si="3"/>
-        <v>4601.2609223744294</v>
-      </c>
-      <c r="D29" s="30">
-        <f t="shared" si="3"/>
-        <v>9205.9788401826499</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>diesel</v>
-      </c>
-      <c r="B30" s="31">
-        <f t="shared" ref="B30:D30" si="4">B26*$H$2*$H6</f>
-        <v>3584.9042648401823</v>
-      </c>
-      <c r="C30" s="31">
+        <v>156</v>
+      </c>
+      <c r="B26" s="54">
+        <f>MeOH_original_data!B23*1000/(24)</f>
+        <v>837.5</v>
+      </c>
+      <c r="C26" s="54">
+        <f>MeOH_original_data!C23*1000/(24)</f>
+        <v>4179.166666666667</v>
+      </c>
+      <c r="D26" s="27">
+        <f>MeOH_original_data!D23*1000/(24)</f>
+        <v>8362.5</v>
+      </c>
+      <c r="F26" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" s="65">
         <f t="shared" si="4"/>
-        <v>17913.502151255707</v>
-      </c>
-      <c r="D30" s="32">
-        <f t="shared" si="4"/>
-        <v>35830.677360159818</v>
+        <v>1.4896551724137932</v>
+      </c>
+      <c r="H26" s="65">
+        <f t="shared" si="5"/>
+        <v>1.4838487972508592</v>
+      </c>
+      <c r="I26" s="66">
+        <f t="shared" si="6"/>
+        <v>1.481303602058319</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="55">
+        <f>MeOH_original_data!B24*1000/(24)</f>
+        <v>3600</v>
+      </c>
+      <c r="C27" s="55">
+        <f>MeOH_original_data!C24*1000/(24)</f>
+        <v>17991.666666666668</v>
+      </c>
+      <c r="D27" s="56">
+        <f>MeOH_original_data!D24*1000/(24)</f>
+        <v>35983.333333333336</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31">
+        <v>100</v>
+      </c>
+      <c r="C31">
+        <v>500</v>
+      </c>
+      <c r="D31">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32">
+        <v>167921429.192</v>
+      </c>
+      <c r="C32">
+        <v>376933297.796</v>
+      </c>
+      <c r="D32">
+        <v>655027563.25600004</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" t="s">
         <v>171</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>100</v>
+      </c>
+      <c r="B34">
+        <v>167921429.192</v>
+      </c>
+      <c r="C34">
+        <f>LN(A34/$A$36)</f>
+        <v>-2.3025850929940455</v>
+      </c>
+      <c r="D34">
+        <f>LN(B34)</f>
+        <v>18.939006744588596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>500</v>
+      </c>
+      <c r="B35">
+        <v>376933297.796</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:C36" si="7">LN(A35/$A$36)</f>
+        <v>-0.69314718055994529</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:D36" si="8">LN(B35)</f>
+        <v>19.747578800835441</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1000</v>
+      </c>
+      <c r="B36">
+        <v>655027563.25600004</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="8"/>
+        <v>20.300187874021002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>142</v>
-      </c>
-      <c r="B34">
-        <v>100</v>
-      </c>
-      <c r="C34">
-        <v>500</v>
-      </c>
-      <c r="D34">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35">
-        <v>167921429.192</v>
-      </c>
-      <c r="C35">
-        <v>376933297.796</v>
-      </c>
-      <c r="D35">
-        <v>655027563.25600004</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>142</v>
-      </c>
-      <c r="B36" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="D36" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>100</v>
-      </c>
-      <c r="B37">
-        <v>167921429.192</v>
-      </c>
-      <c r="C37">
-        <f>LN(A37/$A$39)</f>
-        <v>-2.3025850929940455</v>
-      </c>
-      <c r="D37">
-        <f>LN(B37)</f>
-        <v>18.939006744588596</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>500</v>
-      </c>
-      <c r="B38">
-        <v>376933297.796</v>
-      </c>
-      <c r="C38">
-        <f t="shared" ref="C38:C39" si="5">LN(A38/$A$39)</f>
-        <v>-0.69314718055994529</v>
-      </c>
-      <c r="D38">
-        <f t="shared" ref="D38:D39" si="6">LN(B38)</f>
-        <v>19.747578800835441</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>1000</v>
-      </c>
-      <c r="B39">
-        <v>655027563.25600004</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="6"/>
-        <v>20.300187874021002</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="B42" s="22">
+      <c r="B39" s="22">
         <f>EXP(20.237)</f>
         <v>614918317.57584751</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="B43" s="22">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="B40" s="22">
         <v>0.57550000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>181</v>
-      </c>
-      <c r="B45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42">
         <f>B19</f>
         <v>100</v>
       </c>
-      <c r="C45">
-        <f t="shared" ref="C45:D45" si="7">C19</f>
+      <c r="C42">
+        <f>C19</f>
         <v>500</v>
       </c>
-      <c r="D45">
-        <f t="shared" si="7"/>
+      <c r="D42">
+        <f>D19</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>180</v>
-      </c>
-      <c r="B46">
-        <f>B21/B45</f>
-        <v>22.260273972602739</v>
-      </c>
-      <c r="C46">
-        <f t="shared" ref="C46:D46" si="8">C21/C45</f>
-        <v>22.260273972602739</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="8"/>
-        <v>22.260273972602739</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>180</v>
-      </c>
-      <c r="B47">
-        <f>B46</f>
-        <v>22.260273972602739</v>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B43">
+        <f>B21/B42</f>
+        <v>24.166666666666664</v>
+      </c>
+      <c r="C43">
+        <f>C21/C42</f>
+        <v>24.25</v>
+      </c>
+      <c r="D43">
+        <f>D21/D42</f>
+        <v>24.291666666666668</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>177</v>
+      </c>
+      <c r="B44">
+        <f>B43</f>
+        <v>24.166666666666664</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4291,10 +4409,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDBD3A5-912B-984E-9A90-BB156C754950}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:D16"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4465,7 +4583,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -4473,78 +4591,92 @@
         <v>144</v>
       </c>
       <c r="B18">
-        <v>19500</v>
+        <v>58</v>
       </c>
       <c r="C18">
-        <v>97500</v>
+        <v>291</v>
       </c>
       <c r="D18">
-        <v>195000</v>
+        <v>583</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B19">
-        <v>117251</v>
+        <v>352</v>
       </c>
       <c r="C19">
-        <v>586201</v>
+        <v>1761</v>
       </c>
       <c r="D19">
-        <v>1172515</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>186</v>
+      </c>
+      <c r="B20">
+        <v>5.5</v>
+      </c>
+      <c r="C20">
+        <v>27</v>
+      </c>
+      <c r="D20">
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>154</v>
-      </c>
-      <c r="B21">
-        <v>0.62</v>
-      </c>
-      <c r="C21">
-        <v>3.09</v>
-      </c>
-      <c r="D21">
-        <v>6.18</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B22">
-        <v>2.66</v>
+        <v>2.4</v>
       </c>
       <c r="C22">
-        <v>13.31</v>
+        <v>12.2</v>
       </c>
       <c r="D22">
-        <v>26.63</v>
+        <v>24.4</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B23">
-        <v>9.76</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="C23">
-        <v>48.77</v>
+        <v>100.3</v>
       </c>
       <c r="D23">
-        <v>97.55</v>
+        <v>200.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24">
+        <v>86.4</v>
+      </c>
+      <c r="C24">
+        <v>431.8</v>
+      </c>
+      <c r="D24">
+        <v>863.6</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="63++40v+r24DI1NGDMj3uLvKWHua6+195yfuz655POSYE5c0pg/oxiyqXffUWpeNHnzSmPAPAZtZC71/VoVO3A==" saltValue="LpuP2HeQ38pYq234+AzyYA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="E5wXOZaLLrrq7SCc6l+P2ZRx9IPEuRyCimf3Z0baz1pnEGajuwEnyXDqCBaOzjtZXMtVpsqDvw4pp6yfyAXdcg==" saltValue="DJDNe6oto2IcuT0txsQDEg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
model data for SMR and LWR+MeOH with sweep values sheets to automatically write inputs
</commit_message>
<xml_diff>
--- a/use_cases/LWR_MeOH_2023/data/HERON_data.xlsx
+++ b/use_cases/LWR_MeOH_2023/data/HERON_data.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWR_MeOH_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4689BC62-852B-A848-96A1-302D3FD5988E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB805E72-8AE5-C143-B931-873DC120F73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="2" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="-300" yWindow="880" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sweep values" sheetId="10" r:id="rId1"/>
-    <sheet name="MACRS" sheetId="1" r:id="rId2"/>
-    <sheet name="MeOH" sheetId="14" r:id="rId3"/>
-    <sheet name="MeOH_original_data" sheetId="13" r:id="rId4"/>
-    <sheet name="HTSE" sheetId="2" r:id="rId5"/>
-    <sheet name="Capacity_Market" sheetId="3" r:id="rId6"/>
-    <sheet name="NPP_capacities" sheetId="12" r:id="rId7"/>
+    <sheet name="storage_steps" sheetId="17" r:id="rId2"/>
+    <sheet name="MeOH_steps" sheetId="16" r:id="rId3"/>
+    <sheet name="HTSE_steps" sheetId="15" r:id="rId4"/>
+    <sheet name="MACRS" sheetId="1" r:id="rId5"/>
+    <sheet name="MeOH" sheetId="14" r:id="rId6"/>
+    <sheet name="MeOH_original_data" sheetId="13" r:id="rId7"/>
+    <sheet name="HTSE" sheetId="2" r:id="rId8"/>
+    <sheet name="Capacity_Market" sheetId="3" r:id="rId9"/>
+    <sheet name="NPP_capacities" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="194">
   <si>
     <t>Source</t>
   </si>
@@ -605,6 +608,24 @@
   </si>
   <si>
     <t>Ratios\Scale(MWe)</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>braidwood</t>
+  </si>
+  <si>
+    <t>cooper</t>
+  </si>
+  <si>
+    <t>davis_besse</t>
+  </si>
+  <si>
+    <t>prairie_island</t>
+  </si>
+  <si>
+    <t>stp</t>
   </si>
 </sst>
 </file>
@@ -614,7 +635,7 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -938,7 +959,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -980,6 +1001,19 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1010,27 +1044,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -2399,7 +2415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
@@ -2564,30 +2580,30 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="45" t="s">
+      <c r="D18" s="59"/>
+      <c r="E18" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="45" t="s">
+      <c r="F18" s="59"/>
+      <c r="G18" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="46"/>
+      <c r="H18" s="59"/>
       <c r="I18" s="31"/>
       <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="44"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="11" t="s">
         <v>74</v>
       </c>
@@ -3622,7 +3638,1134 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5236045A-41A7-AF40-95B6-DBF867B04F6F}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3645</v>
+      </c>
+      <c r="F2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="18">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="J2" s="15">
+        <f>$B$10+I2*(1-$B$10)</f>
+        <v>0.28505000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2817</v>
+      </c>
+      <c r="F3">
+        <v>894</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="18">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15">
+        <f t="shared" ref="J3:J8" si="0">$B$10+I3*(1-$B$10)</f>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3853</v>
+      </c>
+      <c r="F4">
+        <v>1280</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="18">
+        <v>0</v>
+      </c>
+      <c r="J4" s="15">
+        <f t="shared" si="0"/>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3411</v>
+      </c>
+      <c r="F5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="18">
+        <v>8.8400000000000006E-2</v>
+      </c>
+      <c r="J5" s="15">
+        <f t="shared" si="0"/>
+        <v>0.27983599999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1677</v>
+      </c>
+      <c r="F6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" s="18">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="J6" s="15">
+        <f t="shared" si="0"/>
+        <v>0.28742000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2419</v>
+      </c>
+      <c r="F7">
+        <v>769</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="18">
+        <v>7.8100000000000003E-2</v>
+      </c>
+      <c r="J7" s="15">
+        <f t="shared" si="0"/>
+        <v>0.27169900000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3990</v>
+      </c>
+      <c r="F8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H8" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="18">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J8" s="15">
+        <f t="shared" si="0"/>
+        <v>0.24870999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="17">
+        <v>0.21</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="14"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{E420822C-9CB6-0543-ADF1-EDCFE8D5ABAC}"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://en.wikipedia.org/wiki/Davis%E2%80%93Besse_Nuclear_Power_Station" xr:uid="{9110542E-89D6-2D47-BAB0-04E98B13FBF5}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{D1783477-78FF-784B-9A1B-672979000EC5}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{50BD1FBC-1D61-6F40-B26D-85ED74F24A2B}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{3096E627-E5FC-5A4A-BC59-39F664A94478}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{A9BD79D7-5527-A44C-B2EE-3F868C0E23D5}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{9DA2C91F-A18F-F04F-A835-EC8502AD4D48}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999CF170-3B2F-5A4A-A635-8F248BA69D8B}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="34">
+        <v>10</v>
+      </c>
+      <c r="C2" s="34">
+        <f>'Sweep values'!C44</f>
+        <v>128888.88888888889</v>
+      </c>
+      <c r="D2" s="34">
+        <f>'Sweep values'!D44</f>
+        <v>257777.77777777778</v>
+      </c>
+      <c r="E2" s="34">
+        <f>'Sweep values'!E44</f>
+        <v>386666.66666666669</v>
+      </c>
+      <c r="F2" s="34">
+        <f>'Sweep values'!F44</f>
+        <v>515555.55555555556</v>
+      </c>
+      <c r="G2" s="34">
+        <f>'Sweep values'!G44</f>
+        <v>644444.4444444445</v>
+      </c>
+      <c r="H2" s="34">
+        <f>'Sweep values'!H44</f>
+        <v>773333.33333333337</v>
+      </c>
+      <c r="I2" s="34">
+        <f>'Sweep values'!I44</f>
+        <v>902222.22222222225</v>
+      </c>
+      <c r="J2" s="34">
+        <f>'Sweep values'!J44</f>
+        <v>1031111.1111111111</v>
+      </c>
+      <c r="K2" s="34">
+        <f>'Sweep values'!K44</f>
+        <v>1160000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="34">
+        <v>10</v>
+      </c>
+      <c r="C3" s="34">
+        <f>'Sweep values'!C45</f>
+        <v>346904.44444444438</v>
+      </c>
+      <c r="D3" s="34">
+        <f>'Sweep values'!D45</f>
+        <v>693808.88888888876</v>
+      </c>
+      <c r="E3" s="34">
+        <f>'Sweep values'!E45</f>
+        <v>1040713.3333333331</v>
+      </c>
+      <c r="F3" s="34">
+        <f>'Sweep values'!F45</f>
+        <v>1387617.7777777775</v>
+      </c>
+      <c r="G3" s="34">
+        <f>'Sweep values'!G45</f>
+        <v>1734522.222222222</v>
+      </c>
+      <c r="H3" s="34">
+        <f>'Sweep values'!H45</f>
+        <v>2081426.6666666663</v>
+      </c>
+      <c r="I3" s="34">
+        <f>'Sweep values'!I45</f>
+        <v>2428331.1111111105</v>
+      </c>
+      <c r="J3" s="34">
+        <f>'Sweep values'!J45</f>
+        <v>2775235.555555555</v>
+      </c>
+      <c r="K3" s="34">
+        <f>'Sweep values'!K45</f>
+        <v>3122139.9999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="34">
+        <v>10</v>
+      </c>
+      <c r="C4" s="34">
+        <f>'Sweep values'!C46</f>
+        <v>115226.66666666664</v>
+      </c>
+      <c r="D4" s="34">
+        <f>'Sweep values'!D46</f>
+        <v>230453.33333333328</v>
+      </c>
+      <c r="E4" s="34">
+        <f>'Sweep values'!E46</f>
+        <v>345679.99999999988</v>
+      </c>
+      <c r="F4" s="34">
+        <f>'Sweep values'!F46</f>
+        <v>460906.66666666657</v>
+      </c>
+      <c r="G4" s="34">
+        <f>'Sweep values'!G46</f>
+        <v>576133.33333333326</v>
+      </c>
+      <c r="H4" s="34">
+        <f>'Sweep values'!H46</f>
+        <v>691359.99999999977</v>
+      </c>
+      <c r="I4" s="34">
+        <f>'Sweep values'!I46</f>
+        <v>806586.66666666651</v>
+      </c>
+      <c r="J4" s="34">
+        <f>'Sweep values'!J46</f>
+        <v>921813.33333333314</v>
+      </c>
+      <c r="K4" s="34">
+        <f>'Sweep values'!K46</f>
+        <v>1037039.9999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="34">
+        <v>10</v>
+      </c>
+      <c r="C5" s="34">
+        <f>'Sweep values'!C47</f>
+        <v>33639.999999999993</v>
+      </c>
+      <c r="D5" s="34">
+        <f>'Sweep values'!D47</f>
+        <v>67279.999999999985</v>
+      </c>
+      <c r="E5" s="34">
+        <f>'Sweep values'!E47</f>
+        <v>100919.99999999997</v>
+      </c>
+      <c r="F5" s="34">
+        <f>'Sweep values'!F47</f>
+        <v>134559.99999999997</v>
+      </c>
+      <c r="G5" s="34">
+        <f>'Sweep values'!G47</f>
+        <v>168199.99999999997</v>
+      </c>
+      <c r="H5" s="34">
+        <f>'Sweep values'!H47</f>
+        <v>201839.99999999994</v>
+      </c>
+      <c r="I5" s="34">
+        <f>'Sweep values'!I47</f>
+        <v>235479.99999999994</v>
+      </c>
+      <c r="J5" s="34">
+        <f>'Sweep values'!J47</f>
+        <v>269119.99999999994</v>
+      </c>
+      <c r="K5" s="34">
+        <f>'Sweep values'!K47</f>
+        <v>302759.99999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="34">
+        <v>10</v>
+      </c>
+      <c r="C6" s="34">
+        <f>'Sweep values'!C48</f>
+        <v>902222.22222222225</v>
+      </c>
+      <c r="D6" s="34">
+        <f>'Sweep values'!D48</f>
+        <v>1804444.4444444445</v>
+      </c>
+      <c r="E6" s="34">
+        <f>'Sweep values'!E48</f>
+        <v>2706666.6666666665</v>
+      </c>
+      <c r="F6" s="34">
+        <f>'Sweep values'!F48</f>
+        <v>3608888.888888889</v>
+      </c>
+      <c r="G6" s="34">
+        <f>'Sweep values'!G48</f>
+        <v>4511111.111111111</v>
+      </c>
+      <c r="H6" s="34">
+        <f>'Sweep values'!H48</f>
+        <v>5413333.333333333</v>
+      </c>
+      <c r="I6" s="34">
+        <f>'Sweep values'!I48</f>
+        <v>6315555.555555556</v>
+      </c>
+      <c r="J6" s="34">
+        <f>'Sweep values'!J48</f>
+        <v>7217777.777777778</v>
+      </c>
+      <c r="K6" s="34">
+        <f>'Sweep values'!K48</f>
+        <v>8120000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="34"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D546BDAA-9A2B-B347-BAD4-55130E108AD7}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="34">
+        <f>'Sweep values'!B36</f>
+        <v>-24166.666666666664</v>
+      </c>
+      <c r="C2" s="34">
+        <f>'Sweep values'!C36</f>
+        <v>-21750</v>
+      </c>
+      <c r="D2" s="34">
+        <f>'Sweep values'!D36</f>
+        <v>-19333.333333333332</v>
+      </c>
+      <c r="E2" s="34">
+        <f>'Sweep values'!E36</f>
+        <v>-16916.666666666664</v>
+      </c>
+      <c r="F2" s="34">
+        <f>'Sweep values'!F36</f>
+        <v>-14500</v>
+      </c>
+      <c r="G2" s="34">
+        <f>'Sweep values'!G36</f>
+        <v>-12083.333333333332</v>
+      </c>
+      <c r="H2" s="34">
+        <f>'Sweep values'!H36</f>
+        <v>-9666.6666666666679</v>
+      </c>
+      <c r="I2" s="34">
+        <f>'Sweep values'!I36</f>
+        <v>-7250</v>
+      </c>
+      <c r="J2" s="34">
+        <f>'Sweep values'!J36</f>
+        <v>-4833.3333333333358</v>
+      </c>
+      <c r="K2" s="34">
+        <f>'Sweep values'!K36</f>
+        <v>-2416.6666666666679</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="34">
+        <f>'Sweep values'!B37</f>
+        <v>-18584.166666666664</v>
+      </c>
+      <c r="C3" s="34">
+        <f>'Sweep values'!C37</f>
+        <v>-16787.777777777774</v>
+      </c>
+      <c r="D3" s="34">
+        <f>'Sweep values'!D37</f>
+        <v>-14991.388888888887</v>
+      </c>
+      <c r="E3" s="34">
+        <f>'Sweep values'!E37</f>
+        <v>-13194.999999999998</v>
+      </c>
+      <c r="F3" s="34">
+        <f>'Sweep values'!F37</f>
+        <v>-11398.611111111109</v>
+      </c>
+      <c r="G3" s="34">
+        <f>'Sweep values'!G37</f>
+        <v>-9602.2222222222208</v>
+      </c>
+      <c r="H3" s="34">
+        <f>'Sweep values'!H37</f>
+        <v>-7805.8333333333321</v>
+      </c>
+      <c r="I3" s="34">
+        <f>'Sweep values'!I37</f>
+        <v>-6009.4444444444434</v>
+      </c>
+      <c r="J3" s="34">
+        <f>'Sweep values'!J37</f>
+        <v>-4213.0555555555547</v>
+      </c>
+      <c r="K3" s="34">
+        <f>'Sweep values'!K37</f>
+        <v>-2416.6666666666679</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="34">
+        <f>'Sweep values'!B38</f>
+        <v>-21604.999999999996</v>
+      </c>
+      <c r="C4" s="34">
+        <f>'Sweep values'!C38</f>
+        <v>-19472.96296296296</v>
+      </c>
+      <c r="D4" s="34">
+        <f>'Sweep values'!D38</f>
+        <v>-17340.925925925923</v>
+      </c>
+      <c r="E4" s="34">
+        <f>'Sweep values'!E38</f>
+        <v>-15208.888888888887</v>
+      </c>
+      <c r="F4" s="34">
+        <f>'Sweep values'!F38</f>
+        <v>-13076.85185185185</v>
+      </c>
+      <c r="G4" s="34">
+        <f>'Sweep values'!G38</f>
+        <v>-10944.814814814814</v>
+      </c>
+      <c r="H4" s="34">
+        <f>'Sweep values'!H38</f>
+        <v>-8812.7777777777774</v>
+      </c>
+      <c r="I4" s="34">
+        <f>'Sweep values'!I38</f>
+        <v>-6680.7407407407391</v>
+      </c>
+      <c r="J4" s="34">
+        <f>'Sweep values'!J38</f>
+        <v>-4548.7037037037044</v>
+      </c>
+      <c r="K4" s="34">
+        <f>'Sweep values'!K38</f>
+        <v>-2416.6666666666679</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="34">
+        <f>'Sweep values'!B39</f>
+        <v>-12614.999999999998</v>
+      </c>
+      <c r="C5" s="34">
+        <f>'Sweep values'!C39</f>
+        <v>-11481.85185185185</v>
+      </c>
+      <c r="D5" s="34">
+        <f>'Sweep values'!D39</f>
+        <v>-10348.703703703703</v>
+      </c>
+      <c r="E5" s="34">
+        <f>'Sweep values'!E39</f>
+        <v>-9215.5555555555547</v>
+      </c>
+      <c r="F5" s="34">
+        <f>'Sweep values'!F39</f>
+        <v>-8082.407407407406</v>
+      </c>
+      <c r="G5" s="34">
+        <f>'Sweep values'!G39</f>
+        <v>-6949.2592592592582</v>
+      </c>
+      <c r="H5" s="34">
+        <f>'Sweep values'!H39</f>
+        <v>-5816.1111111111104</v>
+      </c>
+      <c r="I5" s="34">
+        <f>'Sweep values'!I39</f>
+        <v>-4682.9629629629617</v>
+      </c>
+      <c r="J5" s="34">
+        <f>'Sweep values'!J39</f>
+        <v>-3549.8148148148139</v>
+      </c>
+      <c r="K5" s="34">
+        <f>'Sweep values'!K39</f>
+        <v>-2416.6666666666661</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="34">
+        <f>'Sweep values'!B40</f>
+        <v>-24166.666666666664</v>
+      </c>
+      <c r="C6" s="34">
+        <f>'Sweep values'!C40</f>
+        <v>-21750</v>
+      </c>
+      <c r="D6" s="34">
+        <f>'Sweep values'!D40</f>
+        <v>-19333.333333333332</v>
+      </c>
+      <c r="E6" s="34">
+        <f>'Sweep values'!E40</f>
+        <v>-16916.666666666664</v>
+      </c>
+      <c r="F6" s="34">
+        <f>'Sweep values'!F40</f>
+        <v>-14500</v>
+      </c>
+      <c r="G6" s="34">
+        <f>'Sweep values'!G40</f>
+        <v>-12083.333333333332</v>
+      </c>
+      <c r="H6" s="34">
+        <f>'Sweep values'!H40</f>
+        <v>-9666.6666666666679</v>
+      </c>
+      <c r="I6" s="34">
+        <f>'Sweep values'!I40</f>
+        <v>-7250</v>
+      </c>
+      <c r="J6" s="34">
+        <f>'Sweep values'!J40</f>
+        <v>-4833.3333333333358</v>
+      </c>
+      <c r="K6" s="34">
+        <f>'Sweep values'!K40</f>
+        <v>-2416.6666666666679</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2130096-220E-7649-A477-8C79C6C2607D}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="34">
+        <f>'Sweep values'!B28</f>
+        <v>-1000</v>
+      </c>
+      <c r="C2" s="34">
+        <f>'Sweep values'!C28</f>
+        <v>-900</v>
+      </c>
+      <c r="D2" s="34">
+        <f>'Sweep values'!D28</f>
+        <v>-800</v>
+      </c>
+      <c r="E2" s="34">
+        <f>'Sweep values'!E28</f>
+        <v>-700</v>
+      </c>
+      <c r="F2" s="34">
+        <f>'Sweep values'!F28</f>
+        <v>-600</v>
+      </c>
+      <c r="G2" s="34">
+        <f>'Sweep values'!G28</f>
+        <v>-500</v>
+      </c>
+      <c r="H2" s="34">
+        <f>'Sweep values'!H28</f>
+        <v>-400</v>
+      </c>
+      <c r="I2" s="34">
+        <f>'Sweep values'!I28</f>
+        <v>-300</v>
+      </c>
+      <c r="J2" s="34">
+        <f>'Sweep values'!J28</f>
+        <v>-200</v>
+      </c>
+      <c r="K2" s="34">
+        <f>'Sweep values'!K28</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="34">
+        <f>'Sweep values'!B29</f>
+        <v>-769</v>
+      </c>
+      <c r="C3" s="34">
+        <f>'Sweep values'!C29</f>
+        <v>-694.66666666666663</v>
+      </c>
+      <c r="D3" s="34">
+        <f>'Sweep values'!D29</f>
+        <v>-620.33333333333337</v>
+      </c>
+      <c r="E3" s="34">
+        <f>'Sweep values'!E29</f>
+        <v>-546</v>
+      </c>
+      <c r="F3" s="34">
+        <f>'Sweep values'!F29</f>
+        <v>-471.66666666666669</v>
+      </c>
+      <c r="G3" s="34">
+        <f>'Sweep values'!G29</f>
+        <v>-397.33333333333331</v>
+      </c>
+      <c r="H3" s="34">
+        <f>'Sweep values'!H29</f>
+        <v>-323</v>
+      </c>
+      <c r="I3" s="34">
+        <f>'Sweep values'!I29</f>
+        <v>-248.66666666666663</v>
+      </c>
+      <c r="J3" s="34">
+        <f>'Sweep values'!J29</f>
+        <v>-174.33333333333337</v>
+      </c>
+      <c r="K3" s="34">
+        <f>'Sweep values'!K29</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="34">
+        <f>'Sweep values'!B30</f>
+        <v>-894</v>
+      </c>
+      <c r="C4" s="34">
+        <f>'Sweep values'!C30</f>
+        <v>-805.77777777777783</v>
+      </c>
+      <c r="D4" s="34">
+        <f>'Sweep values'!D30</f>
+        <v>-717.55555555555554</v>
+      </c>
+      <c r="E4" s="34">
+        <f>'Sweep values'!E30</f>
+        <v>-629.33333333333326</v>
+      </c>
+      <c r="F4" s="34">
+        <f>'Sweep values'!F30</f>
+        <v>-541.11111111111109</v>
+      </c>
+      <c r="G4" s="34">
+        <f>'Sweep values'!G30</f>
+        <v>-452.88888888888891</v>
+      </c>
+      <c r="H4" s="34">
+        <f>'Sweep values'!H30</f>
+        <v>-364.66666666666663</v>
+      </c>
+      <c r="I4" s="34">
+        <f>'Sweep values'!I30</f>
+        <v>-276.44444444444446</v>
+      </c>
+      <c r="J4" s="34">
+        <f>'Sweep values'!J30</f>
+        <v>-188.22222222222217</v>
+      </c>
+      <c r="K4" s="34">
+        <f>'Sweep values'!K30</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="34">
+        <f>'Sweep values'!B31</f>
+        <v>-522</v>
+      </c>
+      <c r="C5" s="34">
+        <f>'Sweep values'!C31</f>
+        <v>-475.11111111111109</v>
+      </c>
+      <c r="D5" s="34">
+        <f>'Sweep values'!D31</f>
+        <v>-428.22222222222223</v>
+      </c>
+      <c r="E5" s="34">
+        <f>'Sweep values'!E31</f>
+        <v>-381.33333333333337</v>
+      </c>
+      <c r="F5" s="34">
+        <f>'Sweep values'!F31</f>
+        <v>-334.44444444444446</v>
+      </c>
+      <c r="G5" s="34">
+        <f>'Sweep values'!G31</f>
+        <v>-287.55555555555554</v>
+      </c>
+      <c r="H5" s="34">
+        <f>'Sweep values'!H31</f>
+        <v>-240.66666666666669</v>
+      </c>
+      <c r="I5" s="34">
+        <f>'Sweep values'!I31</f>
+        <v>-193.77777777777777</v>
+      </c>
+      <c r="J5" s="34">
+        <f>'Sweep values'!J31</f>
+        <v>-146.88888888888891</v>
+      </c>
+      <c r="K5" s="34">
+        <f>'Sweep values'!K31</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="34">
+        <f>'Sweep values'!B32</f>
+        <v>-1000</v>
+      </c>
+      <c r="C6" s="34">
+        <f>'Sweep values'!C32</f>
+        <v>-900</v>
+      </c>
+      <c r="D6" s="34">
+        <f>'Sweep values'!D32</f>
+        <v>-800</v>
+      </c>
+      <c r="E6" s="34">
+        <f>'Sweep values'!E32</f>
+        <v>-700</v>
+      </c>
+      <c r="F6" s="34">
+        <f>'Sweep values'!F32</f>
+        <v>-600</v>
+      </c>
+      <c r="G6" s="34">
+        <f>'Sweep values'!G32</f>
+        <v>-500</v>
+      </c>
+      <c r="H6" s="34">
+        <f>'Sweep values'!H32</f>
+        <v>-400</v>
+      </c>
+      <c r="I6" s="34">
+        <f>'Sweep values'!I32</f>
+        <v>-300</v>
+      </c>
+      <c r="J6" s="34">
+        <f>'Sweep values'!J32</f>
+        <v>-200</v>
+      </c>
+      <c r="K6" s="34">
+        <f>'Sweep values'!K32</f>
+        <v>-100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17762179-2135-43B7-98DA-D4A6A7868310}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -3648,10 +4791,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="47"/>
+      <c r="B2" s="60"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -3779,11 +4922,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E49A404-39E7-6B45-B584-7FD70EB84AF5}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -4018,13 +5161,13 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="61" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
-      <c r="F20" s="67" t="s">
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
+      <c r="F20" s="51" t="s">
         <v>187</v>
       </c>
       <c r="G20" s="20">
@@ -4038,31 +5181,31 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="B21" s="58">
+      <c r="B21" s="42">
         <f>MeOH_original_data!B18*1000/(24)</f>
         <v>2416.6666666666665</v>
       </c>
-      <c r="C21" s="58">
+      <c r="C21" s="42">
         <f>MeOH_original_data!C18*1000/(24)</f>
         <v>12125</v>
       </c>
-      <c r="D21" s="59">
+      <c r="D21" s="43">
         <f>MeOH_original_data!D18*1000/(24)</f>
         <v>24291.666666666668</v>
       </c>
-      <c r="F21" s="68" t="s">
+      <c r="F21" s="52" t="s">
         <v>144</v>
       </c>
-      <c r="G21" s="63">
+      <c r="G21" s="47">
         <v>1</v>
       </c>
-      <c r="H21" s="63">
+      <c r="H21" s="47">
         <v>1</v>
       </c>
-      <c r="I21" s="64">
+      <c r="I21" s="48">
         <v>1</v>
       </c>
     </row>
@@ -4070,30 +5213,30 @@
       <c r="A22" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B22" s="60">
+      <c r="B22" s="45">
         <f>MeOH_original_data!B19*1000/(24)</f>
         <v>14666.666666666666</v>
       </c>
-      <c r="C22" s="60">
+      <c r="C22" s="45">
         <f>MeOH_original_data!C19*1000/(24)</f>
         <v>73375</v>
       </c>
-      <c r="D22" s="61">
+      <c r="D22" s="46">
         <f>MeOH_original_data!D19*1000/(24)</f>
         <v>146791.66666666666</v>
       </c>
-      <c r="F22" s="68" t="s">
+      <c r="F22" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="G22" s="63">
+      <c r="G22" s="47">
         <f>G$21*B22/B$21</f>
         <v>6.068965517241379</v>
       </c>
-      <c r="H22" s="63">
-        <f t="shared" ref="H22:I26" si="1">H$21*C22/C21</f>
+      <c r="H22" s="47">
+        <f t="shared" ref="H22:I23" si="1">H$21*C22/C21</f>
         <v>6.0515463917525771</v>
       </c>
-      <c r="I22" s="64">
+      <c r="I22" s="48">
         <f>I$21*D22/D21</f>
         <v>6.0428816466552311</v>
       </c>
@@ -4102,85 +5245,85 @@
       <c r="A23" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B23" s="62">
+      <c r="B23" s="44">
         <f>MeOH_original_data!B20</f>
         <v>5.5</v>
       </c>
-      <c r="C23" s="62">
+      <c r="C23" s="44">
         <f>MeOH_original_data!C20</f>
         <v>27</v>
       </c>
-      <c r="D23" s="62">
+      <c r="D23" s="44">
         <f>MeOH_original_data!D20</f>
         <v>53</v>
       </c>
-      <c r="F23" s="68" t="s">
+      <c r="F23" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="G23" s="63">
-        <f t="shared" ref="G23:G26" si="2">G$21*B23/B$21</f>
+      <c r="G23" s="47">
+        <f t="shared" ref="G23" si="2">G$21*B23/B$21</f>
         <v>2.2758620689655173E-3</v>
       </c>
-      <c r="H23" s="63">
+      <c r="H23" s="47">
         <f t="shared" si="1"/>
         <v>3.6797274275979556E-4</v>
       </c>
-      <c r="I23" s="64">
+      <c r="I23" s="48">
         <f t="shared" si="1"/>
         <v>3.6105591825149024E-4</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="46"/>
-      <c r="F24" s="68" t="s">
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="59"/>
+      <c r="F24" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="63">
+      <c r="G24" s="47">
         <f>G$21*B25/B$21</f>
         <v>4.1379310344827586E-2</v>
       </c>
-      <c r="H24" s="63">
+      <c r="H24" s="47">
         <f t="shared" ref="H24:I24" si="3">H$21*C25/C$21</f>
         <v>4.192439862542955E-2</v>
       </c>
-      <c r="I24" s="64">
+      <c r="I24" s="48">
         <f t="shared" si="3"/>
         <v>4.1852487135506003E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="B25" s="52">
+      <c r="B25" s="42">
         <f>MeOH_original_data!B22*1000/(24)</f>
         <v>100</v>
       </c>
-      <c r="C25" s="52">
+      <c r="C25" s="42">
         <f>MeOH_original_data!C22*1000/(24)</f>
         <v>508.33333333333331</v>
       </c>
-      <c r="D25" s="53">
+      <c r="D25" s="43">
         <f>MeOH_original_data!D22*1000/(24)</f>
         <v>1016.6666666666666</v>
       </c>
-      <c r="F25" s="68" t="s">
+      <c r="F25" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="G25" s="63">
+      <c r="G25" s="47">
         <f t="shared" ref="G25:G26" si="4">G$21*B26/B$21</f>
         <v>0.34655172413793106</v>
       </c>
-      <c r="H25" s="63">
+      <c r="H25" s="47">
         <f t="shared" ref="H25:H26" si="5">H$21*C26/C$21</f>
         <v>0.3446735395189004</v>
       </c>
-      <c r="I25" s="64">
+      <c r="I25" s="48">
         <f t="shared" ref="I25:I26" si="6">I$21*D26/D$21</f>
         <v>0.34425385934819897</v>
       </c>
@@ -4189,11 +5332,11 @@
       <c r="A26" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="54">
+      <c r="B26" s="44">
         <f>MeOH_original_data!B23*1000/(24)</f>
         <v>837.5</v>
       </c>
-      <c r="C26" s="54">
+      <c r="C26" s="44">
         <f>MeOH_original_data!C23*1000/(24)</f>
         <v>4179.166666666667</v>
       </c>
@@ -4201,18 +5344,18 @@
         <f>MeOH_original_data!D23*1000/(24)</f>
         <v>8362.5</v>
       </c>
-      <c r="F26" s="69" t="s">
+      <c r="F26" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="G26" s="65">
+      <c r="G26" s="49">
         <f t="shared" si="4"/>
         <v>1.4896551724137932</v>
       </c>
-      <c r="H26" s="65">
+      <c r="H26" s="49">
         <f t="shared" si="5"/>
         <v>1.4838487972508592</v>
       </c>
-      <c r="I26" s="66">
+      <c r="I26" s="50">
         <f t="shared" si="6"/>
         <v>1.481303602058319</v>
       </c>
@@ -4221,15 +5364,15 @@
       <c r="A27" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B27" s="55">
+      <c r="B27" s="45">
         <f>MeOH_original_data!B24*1000/(24)</f>
         <v>3600</v>
       </c>
-      <c r="C27" s="55">
+      <c r="C27" s="45">
         <f>MeOH_original_data!C24*1000/(24)</f>
         <v>17991.666666666668</v>
       </c>
-      <c r="D27" s="56">
+      <c r="D27" s="46">
         <f>MeOH_original_data!D24*1000/(24)</f>
         <v>35983.333333333336</v>
       </c>
@@ -4407,7 +5550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDBD3A5-912B-984E-9A90-BB156C754950}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -4681,7 +5824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0215393-90AE-4217-9780-C6903F6FBFD3}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -4856,7 +5999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -4986,308 +6129,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5236045A-41A7-AF40-95B6-DBF867B04F6F}">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3645</v>
-      </c>
-      <c r="F2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" s="18">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="J2" s="15">
-        <f>$B$10+I2*(1-$B$10)</f>
-        <v>0.28505000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2817</v>
-      </c>
-      <c r="F3">
-        <v>894</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" s="18">
-        <v>0</v>
-      </c>
-      <c r="J3" s="15">
-        <f t="shared" ref="J3:J8" si="0">$B$10+I3*(1-$B$10)</f>
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3853</v>
-      </c>
-      <c r="F4">
-        <v>1280</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I4" s="18">
-        <v>0</v>
-      </c>
-      <c r="J4" s="15">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>3411</v>
-      </c>
-      <c r="F5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5" s="18">
-        <v>8.8400000000000006E-2</v>
-      </c>
-      <c r="J5" s="15">
-        <f t="shared" si="0"/>
-        <v>0.27983599999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>1677</v>
-      </c>
-      <c r="F6" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="H6" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" s="18">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="J6" s="15">
-        <f t="shared" si="0"/>
-        <v>0.28742000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>2419</v>
-      </c>
-      <c r="F7">
-        <v>769</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I7" s="18">
-        <v>7.8100000000000003E-2</v>
-      </c>
-      <c r="J7" s="15">
-        <f t="shared" si="0"/>
-        <v>0.27169900000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>3990</v>
-      </c>
-      <c r="F8" t="s">
-        <v>123</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="H8" t="s">
-        <v>119</v>
-      </c>
-      <c r="I8" s="18">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="J8" s="15">
-        <f t="shared" si="0"/>
-        <v>0.24870999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="17">
-        <v>0.21</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="14"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{E420822C-9CB6-0543-ADF1-EDCFE8D5ABAC}"/>
-    <hyperlink ref="G3" r:id="rId2" display="https://en.wikipedia.org/wiki/Davis%E2%80%93Besse_Nuclear_Power_Station" xr:uid="{9110542E-89D6-2D47-BAB0-04E98B13FBF5}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{D1783477-78FF-784B-9A1B-672979000EC5}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{50BD1FBC-1D61-6F40-B26D-85ED74F24A2B}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{3096E627-E5FC-5A4A-BC59-39F664A94478}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{A9BD79D7-5527-A44C-B2EE-3F868C0E23D5}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{9DA2C91F-A18F-F04F-A835-EC8502AD4D48}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update conversion rates for meoh process
</commit_message>
<xml_diff>
--- a/use_cases/LWR_MeOH_2023/data/HERON_data.xlsx
+++ b/use_cases/LWR_MeOH_2023/data/HERON_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWR_MeOH_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6AB341-C3E2-ED41-834F-4C9C35D27B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2A824C-E8EE-ED45-A4C4-490E518F709E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="1740" windowWidth="35840" windowHeight="20200" activeTab="5" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sweep values" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="198">
   <si>
     <t>Source</t>
   </si>
@@ -626,6 +626,18 @@
   </si>
   <si>
     <t>prairie</t>
+  </si>
+  <si>
+    <t>Fuel products (bbl/d)</t>
+  </si>
+  <si>
+    <t>bbl to liters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jet fuel </t>
+  </si>
+  <si>
+    <t>density (kg/L)</t>
   </si>
 </sst>
 </file>
@@ -1007,9 +1019,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
@@ -1047,6 +1057,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -2415,7 +2427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
@@ -2573,37 +2585,37 @@
       </c>
       <c r="B16">
         <f>MeOH!B44</f>
-        <v>24.166666666666664</v>
+        <v>24.583333333333336</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="D18" s="59"/>
-      <c r="E18" s="58" t="s">
+      <c r="D18" s="57"/>
+      <c r="E18" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="F18" s="59"/>
-      <c r="G18" s="58" t="s">
+      <c r="F18" s="57"/>
+      <c r="G18" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="59"/>
+      <c r="H18" s="57"/>
       <c r="I18" s="31"/>
       <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="57"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="11" t="s">
         <v>74</v>
       </c>
@@ -2646,11 +2658,11 @@
       </c>
       <c r="E20" s="39">
         <f>C20*$B$16</f>
-        <v>-24166.666666666664</v>
+        <v>-24583.333333333336</v>
       </c>
       <c r="F20" s="39">
         <f>D20*$B$16</f>
-        <v>-2416.6666666666665</v>
+        <v>-2458.3333333333335</v>
       </c>
       <c r="G20" s="34">
         <f>0</f>
@@ -2658,7 +2670,7 @@
       </c>
       <c r="H20" s="34">
         <f>ABS(E20)*24*I20</f>
-        <v>1160000</v>
+        <v>1180000</v>
       </c>
       <c r="I20">
         <f t="shared" ref="I20:I22" si="0">ROUNDUP(J20*$I$24/$J$24,0)</f>
@@ -2685,11 +2697,11 @@
       </c>
       <c r="E21" s="39">
         <f t="shared" ref="E21:E24" si="3">C21*$B$16</f>
-        <v>-18584.166666666664</v>
+        <v>-18904.583333333336</v>
       </c>
       <c r="F21" s="39">
         <f t="shared" ref="F21:F24" si="4">D21*$B$16</f>
-        <v>-2416.6666666666665</v>
+        <v>-2458.3333333333335</v>
       </c>
       <c r="G21" s="34">
         <f>0</f>
@@ -2697,7 +2709,7 @@
       </c>
       <c r="H21" s="34">
         <f t="shared" ref="H21:H23" si="5">ABS(E21)*24*I21</f>
-        <v>3122139.9999999995</v>
+        <v>3175970.0000000005</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
@@ -2724,11 +2736,11 @@
       </c>
       <c r="E22" s="39">
         <f t="shared" si="3"/>
-        <v>-21604.999999999996</v>
+        <v>-21977.500000000004</v>
       </c>
       <c r="F22" s="39">
         <f t="shared" si="4"/>
-        <v>-2416.6666666666665</v>
+        <v>-2458.3333333333335</v>
       </c>
       <c r="G22" s="34">
         <f>0</f>
@@ -2736,7 +2748,7 @@
       </c>
       <c r="H22" s="34">
         <f t="shared" si="5"/>
-        <v>1037039.9999999998</v>
+        <v>1054920.0000000002</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
@@ -2763,11 +2775,11 @@
       </c>
       <c r="E23" s="39">
         <f t="shared" si="3"/>
-        <v>-12614.999999999998</v>
+        <v>-12832.500000000002</v>
       </c>
       <c r="F23" s="39">
         <f t="shared" si="4"/>
-        <v>-2416.6666666666665</v>
+        <v>-2458.3333333333335</v>
       </c>
       <c r="G23" s="34">
         <f>0</f>
@@ -2775,7 +2787,7 @@
       </c>
       <c r="H23" s="34">
         <f t="shared" si="5"/>
-        <v>302759.99999999994</v>
+        <v>307980.00000000006</v>
       </c>
       <c r="I23">
         <f>ROUNDUP(J23*$I$24/$J$24,0)</f>
@@ -2802,11 +2814,11 @@
       </c>
       <c r="E24" s="40">
         <f t="shared" si="3"/>
-        <v>-24166.666666666664</v>
+        <v>-24583.333333333336</v>
       </c>
       <c r="F24" s="40">
         <f t="shared" si="4"/>
-        <v>-2416.6666666666665</v>
+        <v>-2458.3333333333335</v>
       </c>
       <c r="G24" s="37">
         <f>0</f>
@@ -2814,7 +2826,7 @@
       </c>
       <c r="H24" s="37">
         <f>ABS(E24)*24*I24</f>
-        <v>8120000</v>
+        <v>8260000</v>
       </c>
       <c r="I24" s="19">
         <v>14</v>
@@ -3137,43 +3149,43 @@
       </c>
       <c r="B36" s="33">
         <f>$E20+B$35*ABS($E20-$F20)/9</f>
-        <v>-24166.666666666664</v>
+        <v>-24583.333333333336</v>
       </c>
       <c r="C36" s="34">
         <f t="shared" ref="C36:K36" si="8">$E20+C$35*ABS($E20-$F20)/9</f>
-        <v>-21750</v>
+        <v>-22125</v>
       </c>
       <c r="D36" s="33">
         <f t="shared" si="8"/>
-        <v>-19333.333333333332</v>
+        <v>-19666.666666666668</v>
       </c>
       <c r="E36" s="34">
         <f t="shared" si="8"/>
-        <v>-16916.666666666664</v>
+        <v>-17208.333333333336</v>
       </c>
       <c r="F36" s="33">
         <f t="shared" si="8"/>
-        <v>-14500</v>
+        <v>-14750</v>
       </c>
       <c r="G36" s="34">
         <f t="shared" si="8"/>
-        <v>-12083.333333333332</v>
+        <v>-12291.666666666668</v>
       </c>
       <c r="H36" s="33">
         <f t="shared" si="8"/>
-        <v>-9666.6666666666679</v>
+        <v>-9833.3333333333321</v>
       </c>
       <c r="I36" s="34">
         <f t="shared" si="8"/>
-        <v>-7250</v>
+        <v>-7375</v>
       </c>
       <c r="J36" s="33">
         <f t="shared" si="8"/>
-        <v>-4833.3333333333358</v>
+        <v>-4916.6666666666642</v>
       </c>
       <c r="K36" s="35">
         <f t="shared" si="8"/>
-        <v>-2416.6666666666679</v>
+        <v>-2458.3333333333321</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3182,43 +3194,43 @@
       </c>
       <c r="B37" s="33">
         <f t="shared" ref="B37:K40" si="9">$E21+B$35*ABS($E21-$F21)/9</f>
-        <v>-18584.166666666664</v>
+        <v>-18904.583333333336</v>
       </c>
       <c r="C37" s="34">
         <f t="shared" si="9"/>
-        <v>-16787.777777777774</v>
+        <v>-17077.222222222223</v>
       </c>
       <c r="D37" s="33">
         <f t="shared" si="9"/>
-        <v>-14991.388888888887</v>
+        <v>-15249.861111111113</v>
       </c>
       <c r="E37" s="34">
         <f t="shared" si="9"/>
-        <v>-13194.999999999998</v>
+        <v>-13422.5</v>
       </c>
       <c r="F37" s="33">
         <f t="shared" si="9"/>
-        <v>-11398.611111111109</v>
+        <v>-11595.138888888891</v>
       </c>
       <c r="G37" s="34">
         <f t="shared" si="9"/>
-        <v>-9602.2222222222208</v>
+        <v>-9767.7777777777792</v>
       </c>
       <c r="H37" s="33">
         <f t="shared" si="9"/>
-        <v>-7805.8333333333321</v>
+        <v>-7940.4166666666661</v>
       </c>
       <c r="I37" s="34">
         <f t="shared" si="9"/>
-        <v>-6009.4444444444434</v>
+        <v>-6113.0555555555547</v>
       </c>
       <c r="J37" s="33">
         <f t="shared" si="9"/>
-        <v>-4213.0555555555547</v>
+        <v>-4285.6944444444434</v>
       </c>
       <c r="K37" s="35">
         <f t="shared" si="9"/>
-        <v>-2416.6666666666679</v>
+        <v>-2458.3333333333321</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3227,43 +3239,43 @@
       </c>
       <c r="B38" s="33">
         <f t="shared" si="9"/>
-        <v>-21604.999999999996</v>
+        <v>-21977.500000000004</v>
       </c>
       <c r="C38" s="34">
         <f t="shared" si="9"/>
-        <v>-19472.96296296296</v>
+        <v>-19808.703703703708</v>
       </c>
       <c r="D38" s="33">
         <f t="shared" si="9"/>
-        <v>-17340.925925925923</v>
+        <v>-17639.907407407409</v>
       </c>
       <c r="E38" s="34">
         <f t="shared" si="9"/>
-        <v>-15208.888888888887</v>
+        <v>-15471.111111111113</v>
       </c>
       <c r="F38" s="33">
         <f t="shared" si="9"/>
-        <v>-13076.85185185185</v>
+        <v>-13302.314814814816</v>
       </c>
       <c r="G38" s="34">
         <f t="shared" si="9"/>
-        <v>-10944.814814814814</v>
+        <v>-11133.51851851852</v>
       </c>
       <c r="H38" s="33">
         <f t="shared" si="9"/>
-        <v>-8812.7777777777774</v>
+        <v>-8964.7222222222226</v>
       </c>
       <c r="I38" s="34">
         <f t="shared" si="9"/>
-        <v>-6680.7407407407391</v>
+        <v>-6795.925925925927</v>
       </c>
       <c r="J38" s="33">
         <f t="shared" si="9"/>
-        <v>-4548.7037037037044</v>
+        <v>-4627.1296296296277</v>
       </c>
       <c r="K38" s="35">
         <f t="shared" si="9"/>
-        <v>-2416.6666666666679</v>
+        <v>-2458.3333333333321</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3272,43 +3284,43 @@
       </c>
       <c r="B39" s="33">
         <f t="shared" si="9"/>
-        <v>-12614.999999999998</v>
+        <v>-12832.500000000002</v>
       </c>
       <c r="C39" s="34">
         <f t="shared" si="9"/>
-        <v>-11481.85185185185</v>
+        <v>-11679.814814814818</v>
       </c>
       <c r="D39" s="33">
         <f t="shared" si="9"/>
-        <v>-10348.703703703703</v>
+        <v>-10527.129629629631</v>
       </c>
       <c r="E39" s="34">
         <f t="shared" si="9"/>
-        <v>-9215.5555555555547</v>
+        <v>-9374.4444444444453</v>
       </c>
       <c r="F39" s="33">
         <f t="shared" si="9"/>
-        <v>-8082.407407407406</v>
+        <v>-8221.7592592592609</v>
       </c>
       <c r="G39" s="34">
         <f t="shared" si="9"/>
-        <v>-6949.2592592592582</v>
+        <v>-7069.0740740740748</v>
       </c>
       <c r="H39" s="33">
         <f t="shared" si="9"/>
-        <v>-5816.1111111111104</v>
+        <v>-5916.3888888888896</v>
       </c>
       <c r="I39" s="34">
         <f t="shared" si="9"/>
-        <v>-4682.9629629629617</v>
+        <v>-4763.7037037037053</v>
       </c>
       <c r="J39" s="33">
         <f t="shared" si="9"/>
-        <v>-3549.8148148148139</v>
+        <v>-3611.0185185185201</v>
       </c>
       <c r="K39" s="35">
         <f t="shared" si="9"/>
-        <v>-2416.6666666666661</v>
+        <v>-2458.3333333333339</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3317,43 +3329,43 @@
       </c>
       <c r="B40" s="36">
         <f t="shared" si="9"/>
-        <v>-24166.666666666664</v>
+        <v>-24583.333333333336</v>
       </c>
       <c r="C40" s="37">
         <f t="shared" si="9"/>
-        <v>-21750</v>
+        <v>-22125</v>
       </c>
       <c r="D40" s="36">
         <f t="shared" si="9"/>
-        <v>-19333.333333333332</v>
+        <v>-19666.666666666668</v>
       </c>
       <c r="E40" s="37">
         <f t="shared" si="9"/>
-        <v>-16916.666666666664</v>
+        <v>-17208.333333333336</v>
       </c>
       <c r="F40" s="36">
         <f t="shared" si="9"/>
-        <v>-14500</v>
+        <v>-14750</v>
       </c>
       <c r="G40" s="37">
         <f t="shared" si="9"/>
-        <v>-12083.333333333332</v>
+        <v>-12291.666666666668</v>
       </c>
       <c r="H40" s="36">
         <f t="shared" si="9"/>
-        <v>-9666.6666666666679</v>
+        <v>-9833.3333333333321</v>
       </c>
       <c r="I40" s="37">
         <f t="shared" si="9"/>
-        <v>-7250</v>
+        <v>-7375</v>
       </c>
       <c r="J40" s="36">
         <f t="shared" si="9"/>
-        <v>-4833.3333333333358</v>
+        <v>-4916.6666666666642</v>
       </c>
       <c r="K40" s="38">
         <f t="shared" si="9"/>
-        <v>-2416.6666666666679</v>
+        <v>-2458.3333333333321</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3406,39 +3418,39 @@
       </c>
       <c r="C44" s="34">
         <f t="shared" ref="C44:J44" si="10">C$43*ABS($G20-$H20)/9</f>
-        <v>128888.88888888889</v>
+        <v>131111.11111111112</v>
       </c>
       <c r="D44" s="33">
         <f t="shared" si="10"/>
-        <v>257777.77777777778</v>
+        <v>262222.22222222225</v>
       </c>
       <c r="E44" s="34">
         <f t="shared" si="10"/>
-        <v>386666.66666666669</v>
+        <v>393333.33333333331</v>
       </c>
       <c r="F44" s="33">
         <f t="shared" si="10"/>
-        <v>515555.55555555556</v>
+        <v>524444.4444444445</v>
       </c>
       <c r="G44" s="34">
         <f t="shared" si="10"/>
-        <v>644444.4444444445</v>
+        <v>655555.5555555555</v>
       </c>
       <c r="H44" s="33">
         <f t="shared" si="10"/>
-        <v>773333.33333333337</v>
+        <v>786666.66666666663</v>
       </c>
       <c r="I44" s="34">
         <f t="shared" si="10"/>
-        <v>902222.22222222225</v>
+        <v>917777.77777777775</v>
       </c>
       <c r="J44" s="33">
         <f t="shared" si="10"/>
-        <v>1031111.1111111111</v>
+        <v>1048888.888888889</v>
       </c>
       <c r="K44" s="35">
         <f>K$43*ABS($G20-$H20)/9</f>
-        <v>1160000</v>
+        <v>1180000</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3451,39 +3463,39 @@
       </c>
       <c r="C45" s="34">
         <f t="shared" si="11"/>
-        <v>346904.44444444438</v>
+        <v>352885.55555555562</v>
       </c>
       <c r="D45" s="33">
         <f t="shared" si="11"/>
-        <v>693808.88888888876</v>
+        <v>705771.11111111124</v>
       </c>
       <c r="E45" s="34">
         <f t="shared" si="11"/>
-        <v>1040713.3333333331</v>
+        <v>1058656.666666667</v>
       </c>
       <c r="F45" s="33">
         <f t="shared" si="11"/>
-        <v>1387617.7777777775</v>
+        <v>1411542.2222222225</v>
       </c>
       <c r="G45" s="34">
         <f t="shared" si="11"/>
-        <v>1734522.222222222</v>
+        <v>1764427.777777778</v>
       </c>
       <c r="H45" s="33">
         <f t="shared" si="11"/>
-        <v>2081426.6666666663</v>
+        <v>2117313.333333334</v>
       </c>
       <c r="I45" s="34">
         <f t="shared" si="11"/>
-        <v>2428331.1111111105</v>
+        <v>2470198.8888888895</v>
       </c>
       <c r="J45" s="33">
         <f t="shared" si="11"/>
-        <v>2775235.555555555</v>
+        <v>2823084.444444445</v>
       </c>
       <c r="K45" s="35">
         <f t="shared" si="11"/>
-        <v>3122139.9999999995</v>
+        <v>3175970.0000000005</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3496,39 +3508,39 @@
       </c>
       <c r="C46" s="34">
         <f t="shared" si="12"/>
-        <v>115226.66666666664</v>
+        <v>117213.33333333336</v>
       </c>
       <c r="D46" s="33">
         <f t="shared" si="12"/>
-        <v>230453.33333333328</v>
+        <v>234426.66666666672</v>
       </c>
       <c r="E46" s="34">
         <f t="shared" si="12"/>
-        <v>345679.99999999988</v>
+        <v>351640.00000000012</v>
       </c>
       <c r="F46" s="33">
         <f t="shared" si="12"/>
-        <v>460906.66666666657</v>
+        <v>468853.33333333343</v>
       </c>
       <c r="G46" s="34">
         <f t="shared" si="12"/>
-        <v>576133.33333333326</v>
+        <v>586066.66666666674</v>
       </c>
       <c r="H46" s="33">
         <f t="shared" si="12"/>
-        <v>691359.99999999977</v>
+        <v>703280.00000000023</v>
       </c>
       <c r="I46" s="34">
         <f t="shared" si="12"/>
-        <v>806586.66666666651</v>
+        <v>820493.33333333349</v>
       </c>
       <c r="J46" s="33">
         <f t="shared" si="12"/>
-        <v>921813.33333333314</v>
+        <v>937706.66666666686</v>
       </c>
       <c r="K46" s="35">
         <f t="shared" si="12"/>
-        <v>1037039.9999999998</v>
+        <v>1054920.0000000002</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3541,39 +3553,39 @@
       </c>
       <c r="C47" s="34">
         <f t="shared" si="13"/>
-        <v>33639.999999999993</v>
+        <v>34220.000000000007</v>
       </c>
       <c r="D47" s="33">
         <f t="shared" si="13"/>
-        <v>67279.999999999985</v>
+        <v>68440.000000000015</v>
       </c>
       <c r="E47" s="34">
         <f t="shared" si="13"/>
-        <v>100919.99999999997</v>
+        <v>102660.00000000003</v>
       </c>
       <c r="F47" s="33">
         <f t="shared" si="13"/>
-        <v>134559.99999999997</v>
+        <v>136880.00000000003</v>
       </c>
       <c r="G47" s="34">
         <f t="shared" si="13"/>
-        <v>168199.99999999997</v>
+        <v>171100.00000000003</v>
       </c>
       <c r="H47" s="33">
         <f t="shared" si="13"/>
-        <v>201839.99999999994</v>
+        <v>205320.00000000006</v>
       </c>
       <c r="I47" s="34">
         <f t="shared" si="13"/>
-        <v>235479.99999999994</v>
+        <v>239540.00000000006</v>
       </c>
       <c r="J47" s="33">
         <f t="shared" si="13"/>
-        <v>269119.99999999994</v>
+        <v>273760.00000000006</v>
       </c>
       <c r="K47" s="35">
         <f t="shared" si="13"/>
-        <v>302759.99999999994</v>
+        <v>307980.00000000006</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3586,39 +3598,39 @@
       </c>
       <c r="C48" s="37">
         <f t="shared" si="14"/>
-        <v>902222.22222222225</v>
+        <v>917777.77777777775</v>
       </c>
       <c r="D48" s="36">
         <f t="shared" si="14"/>
-        <v>1804444.4444444445</v>
+        <v>1835555.5555555555</v>
       </c>
       <c r="E48" s="37">
         <f t="shared" si="14"/>
-        <v>2706666.6666666665</v>
+        <v>2753333.3333333335</v>
       </c>
       <c r="F48" s="36">
         <f t="shared" si="14"/>
-        <v>3608888.888888889</v>
+        <v>3671111.111111111</v>
       </c>
       <c r="G48" s="37">
         <f t="shared" si="14"/>
-        <v>4511111.111111111</v>
+        <v>4588888.888888889</v>
       </c>
       <c r="H48" s="36">
         <f t="shared" si="14"/>
-        <v>5413333.333333333</v>
+        <v>5506666.666666667</v>
       </c>
       <c r="I48" s="37">
         <f t="shared" si="14"/>
-        <v>6315555.555555556</v>
+        <v>6424444.444444444</v>
       </c>
       <c r="J48" s="36">
         <f t="shared" si="14"/>
-        <v>7217777.777777778</v>
+        <v>7342222.222222222</v>
       </c>
       <c r="K48" s="38">
         <f t="shared" si="14"/>
-        <v>8120000</v>
+        <v>8260000</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -3946,7 +3958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999CF170-3B2F-5A4A-A635-8F248BA69D8B}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -3996,39 +4008,39 @@
       </c>
       <c r="C2" s="34">
         <f>'Sweep values'!C44</f>
-        <v>128888.88888888889</v>
+        <v>131111.11111111112</v>
       </c>
       <c r="D2" s="34">
         <f>'Sweep values'!D44</f>
-        <v>257777.77777777778</v>
+        <v>262222.22222222225</v>
       </c>
       <c r="E2" s="34">
         <f>'Sweep values'!E44</f>
-        <v>386666.66666666669</v>
+        <v>393333.33333333331</v>
       </c>
       <c r="F2" s="34">
         <f>'Sweep values'!F44</f>
-        <v>515555.55555555556</v>
+        <v>524444.4444444445</v>
       </c>
       <c r="G2" s="34">
         <f>'Sweep values'!G44</f>
-        <v>644444.4444444445</v>
+        <v>655555.5555555555</v>
       </c>
       <c r="H2" s="34">
         <f>'Sweep values'!H44</f>
-        <v>773333.33333333337</v>
+        <v>786666.66666666663</v>
       </c>
       <c r="I2" s="34">
         <f>'Sweep values'!I44</f>
-        <v>902222.22222222225</v>
+        <v>917777.77777777775</v>
       </c>
       <c r="J2" s="34">
         <f>'Sweep values'!J44</f>
-        <v>1031111.1111111111</v>
+        <v>1048888.888888889</v>
       </c>
       <c r="K2" s="34">
         <f>'Sweep values'!K44</f>
-        <v>1160000</v>
+        <v>1180000</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -4040,39 +4052,39 @@
       </c>
       <c r="C3" s="34">
         <f>'Sweep values'!C45</f>
-        <v>346904.44444444438</v>
+        <v>352885.55555555562</v>
       </c>
       <c r="D3" s="34">
         <f>'Sweep values'!D45</f>
-        <v>693808.88888888876</v>
+        <v>705771.11111111124</v>
       </c>
       <c r="E3" s="34">
         <f>'Sweep values'!E45</f>
-        <v>1040713.3333333331</v>
+        <v>1058656.666666667</v>
       </c>
       <c r="F3" s="34">
         <f>'Sweep values'!F45</f>
-        <v>1387617.7777777775</v>
+        <v>1411542.2222222225</v>
       </c>
       <c r="G3" s="34">
         <f>'Sweep values'!G45</f>
-        <v>1734522.222222222</v>
+        <v>1764427.777777778</v>
       </c>
       <c r="H3" s="34">
         <f>'Sweep values'!H45</f>
-        <v>2081426.6666666663</v>
+        <v>2117313.333333334</v>
       </c>
       <c r="I3" s="34">
         <f>'Sweep values'!I45</f>
-        <v>2428331.1111111105</v>
+        <v>2470198.8888888895</v>
       </c>
       <c r="J3" s="34">
         <f>'Sweep values'!J45</f>
-        <v>2775235.555555555</v>
+        <v>2823084.444444445</v>
       </c>
       <c r="K3" s="34">
         <f>'Sweep values'!K45</f>
-        <v>3122139.9999999995</v>
+        <v>3175970.0000000005</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -4084,39 +4096,39 @@
       </c>
       <c r="C4" s="34">
         <f>'Sweep values'!C46</f>
-        <v>115226.66666666664</v>
+        <v>117213.33333333336</v>
       </c>
       <c r="D4" s="34">
         <f>'Sweep values'!D46</f>
-        <v>230453.33333333328</v>
+        <v>234426.66666666672</v>
       </c>
       <c r="E4" s="34">
         <f>'Sweep values'!E46</f>
-        <v>345679.99999999988</v>
+        <v>351640.00000000012</v>
       </c>
       <c r="F4" s="34">
         <f>'Sweep values'!F46</f>
-        <v>460906.66666666657</v>
+        <v>468853.33333333343</v>
       </c>
       <c r="G4" s="34">
         <f>'Sweep values'!G46</f>
-        <v>576133.33333333326</v>
+        <v>586066.66666666674</v>
       </c>
       <c r="H4" s="34">
         <f>'Sweep values'!H46</f>
-        <v>691359.99999999977</v>
+        <v>703280.00000000023</v>
       </c>
       <c r="I4" s="34">
         <f>'Sweep values'!I46</f>
-        <v>806586.66666666651</v>
+        <v>820493.33333333349</v>
       </c>
       <c r="J4" s="34">
         <f>'Sweep values'!J46</f>
-        <v>921813.33333333314</v>
+        <v>937706.66666666686</v>
       </c>
       <c r="K4" s="34">
         <f>'Sweep values'!K46</f>
-        <v>1037039.9999999998</v>
+        <v>1054920.0000000002</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -4128,39 +4140,39 @@
       </c>
       <c r="C5" s="34">
         <f>'Sweep values'!C47</f>
-        <v>33639.999999999993</v>
+        <v>34220.000000000007</v>
       </c>
       <c r="D5" s="34">
         <f>'Sweep values'!D47</f>
-        <v>67279.999999999985</v>
+        <v>68440.000000000015</v>
       </c>
       <c r="E5" s="34">
         <f>'Sweep values'!E47</f>
-        <v>100919.99999999997</v>
+        <v>102660.00000000003</v>
       </c>
       <c r="F5" s="34">
         <f>'Sweep values'!F47</f>
-        <v>134559.99999999997</v>
+        <v>136880.00000000003</v>
       </c>
       <c r="G5" s="34">
         <f>'Sweep values'!G47</f>
-        <v>168199.99999999997</v>
+        <v>171100.00000000003</v>
       </c>
       <c r="H5" s="34">
         <f>'Sweep values'!H47</f>
-        <v>201839.99999999994</v>
+        <v>205320.00000000006</v>
       </c>
       <c r="I5" s="34">
         <f>'Sweep values'!I47</f>
-        <v>235479.99999999994</v>
+        <v>239540.00000000006</v>
       </c>
       <c r="J5" s="34">
         <f>'Sweep values'!J47</f>
-        <v>269119.99999999994</v>
+        <v>273760.00000000006</v>
       </c>
       <c r="K5" s="34">
         <f>'Sweep values'!K47</f>
-        <v>302759.99999999994</v>
+        <v>307980.00000000006</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -4172,39 +4184,39 @@
       </c>
       <c r="C6" s="34">
         <f>'Sweep values'!C48</f>
-        <v>902222.22222222225</v>
+        <v>917777.77777777775</v>
       </c>
       <c r="D6" s="34">
         <f>'Sweep values'!D48</f>
-        <v>1804444.4444444445</v>
+        <v>1835555.5555555555</v>
       </c>
       <c r="E6" s="34">
         <f>'Sweep values'!E48</f>
-        <v>2706666.6666666665</v>
+        <v>2753333.3333333335</v>
       </c>
       <c r="F6" s="34">
         <f>'Sweep values'!F48</f>
-        <v>3608888.888888889</v>
+        <v>3671111.111111111</v>
       </c>
       <c r="G6" s="34">
         <f>'Sweep values'!G48</f>
-        <v>4511111.111111111</v>
+        <v>4588888.888888889</v>
       </c>
       <c r="H6" s="34">
         <f>'Sweep values'!H48</f>
-        <v>5413333.333333333</v>
+        <v>5506666.666666667</v>
       </c>
       <c r="I6" s="34">
         <f>'Sweep values'!I48</f>
-        <v>6315555.555555556</v>
+        <v>6424444.444444444</v>
       </c>
       <c r="J6" s="34">
         <f>'Sweep values'!J48</f>
-        <v>7217777.777777778</v>
+        <v>7342222.222222222</v>
       </c>
       <c r="K6" s="34">
         <f>'Sweep values'!K48</f>
-        <v>8120000</v>
+        <v>8260000</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -4266,43 +4278,43 @@
       </c>
       <c r="B2" s="34">
         <f>'Sweep values'!B36</f>
-        <v>-24166.666666666664</v>
+        <v>-24583.333333333336</v>
       </c>
       <c r="C2" s="34">
         <f>'Sweep values'!C36</f>
-        <v>-21750</v>
+        <v>-22125</v>
       </c>
       <c r="D2" s="34">
         <f>'Sweep values'!D36</f>
-        <v>-19333.333333333332</v>
+        <v>-19666.666666666668</v>
       </c>
       <c r="E2" s="34">
         <f>'Sweep values'!E36</f>
-        <v>-16916.666666666664</v>
+        <v>-17208.333333333336</v>
       </c>
       <c r="F2" s="34">
         <f>'Sweep values'!F36</f>
-        <v>-14500</v>
+        <v>-14750</v>
       </c>
       <c r="G2" s="34">
         <f>'Sweep values'!G36</f>
-        <v>-12083.333333333332</v>
+        <v>-12291.666666666668</v>
       </c>
       <c r="H2" s="34">
         <f>'Sweep values'!H36</f>
-        <v>-9666.6666666666679</v>
+        <v>-9833.3333333333321</v>
       </c>
       <c r="I2" s="34">
         <f>'Sweep values'!I36</f>
-        <v>-7250</v>
+        <v>-7375</v>
       </c>
       <c r="J2" s="34">
         <f>'Sweep values'!J36</f>
-        <v>-4833.3333333333358</v>
+        <v>-4916.6666666666642</v>
       </c>
       <c r="K2" s="34">
         <f>'Sweep values'!K36</f>
-        <v>-2416.6666666666679</v>
+        <v>-2458.3333333333321</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -4311,43 +4323,43 @@
       </c>
       <c r="B3" s="34">
         <f>'Sweep values'!B37</f>
-        <v>-18584.166666666664</v>
+        <v>-18904.583333333336</v>
       </c>
       <c r="C3" s="34">
         <f>'Sweep values'!C37</f>
-        <v>-16787.777777777774</v>
+        <v>-17077.222222222223</v>
       </c>
       <c r="D3" s="34">
         <f>'Sweep values'!D37</f>
-        <v>-14991.388888888887</v>
+        <v>-15249.861111111113</v>
       </c>
       <c r="E3" s="34">
         <f>'Sweep values'!E37</f>
-        <v>-13194.999999999998</v>
+        <v>-13422.5</v>
       </c>
       <c r="F3" s="34">
         <f>'Sweep values'!F37</f>
-        <v>-11398.611111111109</v>
+        <v>-11595.138888888891</v>
       </c>
       <c r="G3" s="34">
         <f>'Sweep values'!G37</f>
-        <v>-9602.2222222222208</v>
+        <v>-9767.7777777777792</v>
       </c>
       <c r="H3" s="34">
         <f>'Sweep values'!H37</f>
-        <v>-7805.8333333333321</v>
+        <v>-7940.4166666666661</v>
       </c>
       <c r="I3" s="34">
         <f>'Sweep values'!I37</f>
-        <v>-6009.4444444444434</v>
+        <v>-6113.0555555555547</v>
       </c>
       <c r="J3" s="34">
         <f>'Sweep values'!J37</f>
-        <v>-4213.0555555555547</v>
+        <v>-4285.6944444444434</v>
       </c>
       <c r="K3" s="34">
         <f>'Sweep values'!K37</f>
-        <v>-2416.6666666666679</v>
+        <v>-2458.3333333333321</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -4356,43 +4368,43 @@
       </c>
       <c r="B4" s="34">
         <f>'Sweep values'!B38</f>
-        <v>-21604.999999999996</v>
+        <v>-21977.500000000004</v>
       </c>
       <c r="C4" s="34">
         <f>'Sweep values'!C38</f>
-        <v>-19472.96296296296</v>
+        <v>-19808.703703703708</v>
       </c>
       <c r="D4" s="34">
         <f>'Sweep values'!D38</f>
-        <v>-17340.925925925923</v>
+        <v>-17639.907407407409</v>
       </c>
       <c r="E4" s="34">
         <f>'Sweep values'!E38</f>
-        <v>-15208.888888888887</v>
+        <v>-15471.111111111113</v>
       </c>
       <c r="F4" s="34">
         <f>'Sweep values'!F38</f>
-        <v>-13076.85185185185</v>
+        <v>-13302.314814814816</v>
       </c>
       <c r="G4" s="34">
         <f>'Sweep values'!G38</f>
-        <v>-10944.814814814814</v>
+        <v>-11133.51851851852</v>
       </c>
       <c r="H4" s="34">
         <f>'Sweep values'!H38</f>
-        <v>-8812.7777777777774</v>
+        <v>-8964.7222222222226</v>
       </c>
       <c r="I4" s="34">
         <f>'Sweep values'!I38</f>
-        <v>-6680.7407407407391</v>
+        <v>-6795.925925925927</v>
       </c>
       <c r="J4" s="34">
         <f>'Sweep values'!J38</f>
-        <v>-4548.7037037037044</v>
+        <v>-4627.1296296296277</v>
       </c>
       <c r="K4" s="34">
         <f>'Sweep values'!K38</f>
-        <v>-2416.6666666666679</v>
+        <v>-2458.3333333333321</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -4401,43 +4413,43 @@
       </c>
       <c r="B5" s="34">
         <f>'Sweep values'!B39</f>
-        <v>-12614.999999999998</v>
+        <v>-12832.500000000002</v>
       </c>
       <c r="C5" s="34">
         <f>'Sweep values'!C39</f>
-        <v>-11481.85185185185</v>
+        <v>-11679.814814814818</v>
       </c>
       <c r="D5" s="34">
         <f>'Sweep values'!D39</f>
-        <v>-10348.703703703703</v>
+        <v>-10527.129629629631</v>
       </c>
       <c r="E5" s="34">
         <f>'Sweep values'!E39</f>
-        <v>-9215.5555555555547</v>
+        <v>-9374.4444444444453</v>
       </c>
       <c r="F5" s="34">
         <f>'Sweep values'!F39</f>
-        <v>-8082.407407407406</v>
+        <v>-8221.7592592592609</v>
       </c>
       <c r="G5" s="34">
         <f>'Sweep values'!G39</f>
-        <v>-6949.2592592592582</v>
+        <v>-7069.0740740740748</v>
       </c>
       <c r="H5" s="34">
         <f>'Sweep values'!H39</f>
-        <v>-5816.1111111111104</v>
+        <v>-5916.3888888888896</v>
       </c>
       <c r="I5" s="34">
         <f>'Sweep values'!I39</f>
-        <v>-4682.9629629629617</v>
+        <v>-4763.7037037037053</v>
       </c>
       <c r="J5" s="34">
         <f>'Sweep values'!J39</f>
-        <v>-3549.8148148148139</v>
+        <v>-3611.0185185185201</v>
       </c>
       <c r="K5" s="34">
         <f>'Sweep values'!K39</f>
-        <v>-2416.6666666666661</v>
+        <v>-2458.3333333333339</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -4446,43 +4458,43 @@
       </c>
       <c r="B6" s="34">
         <f>'Sweep values'!B40</f>
-        <v>-24166.666666666664</v>
+        <v>-24583.333333333336</v>
       </c>
       <c r="C6" s="34">
         <f>'Sweep values'!C40</f>
-        <v>-21750</v>
+        <v>-22125</v>
       </c>
       <c r="D6" s="34">
         <f>'Sweep values'!D40</f>
-        <v>-19333.333333333332</v>
+        <v>-19666.666666666668</v>
       </c>
       <c r="E6" s="34">
         <f>'Sweep values'!E40</f>
-        <v>-16916.666666666664</v>
+        <v>-17208.333333333336</v>
       </c>
       <c r="F6" s="34">
         <f>'Sweep values'!F40</f>
-        <v>-14500</v>
+        <v>-14750</v>
       </c>
       <c r="G6" s="34">
         <f>'Sweep values'!G40</f>
-        <v>-12083.333333333332</v>
+        <v>-12291.666666666668</v>
       </c>
       <c r="H6" s="34">
         <f>'Sweep values'!H40</f>
-        <v>-9666.6666666666679</v>
+        <v>-9833.3333333333321</v>
       </c>
       <c r="I6" s="34">
         <f>'Sweep values'!I40</f>
-        <v>-7250</v>
+        <v>-7375</v>
       </c>
       <c r="J6" s="34">
         <f>'Sweep values'!J40</f>
-        <v>-4833.3333333333358</v>
+        <v>-4916.6666666666642</v>
       </c>
       <c r="K6" s="34">
         <f>'Sweep values'!K40</f>
-        <v>-2416.6666666666679</v>
+        <v>-2458.3333333333321</v>
       </c>
     </row>
   </sheetData>
@@ -4791,10 +4803,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="60"/>
+      <c r="B2" s="58"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -4926,8 +4938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E49A404-39E7-6B45-B584-7FD70EB84AF5}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5161,13 +5173,13 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="59" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
-      <c r="F20" s="51" t="s">
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="61"/>
+      <c r="F20" s="49" t="s">
         <v>187</v>
       </c>
       <c r="G20" s="20">
@@ -5186,26 +5198,26 @@
       </c>
       <c r="B21" s="42">
         <f>MeOH_original_data!B18*1000/(24)</f>
-        <v>2416.6666666666665</v>
+        <v>2458.3333333333335</v>
       </c>
       <c r="C21" s="42">
         <f>MeOH_original_data!C18*1000/(24)</f>
-        <v>12125</v>
+        <v>12208.333333333334</v>
       </c>
       <c r="D21" s="43">
         <f>MeOH_original_data!D18*1000/(24)</f>
-        <v>24291.666666666668</v>
-      </c>
-      <c r="F21" s="52" t="s">
+        <v>24375</v>
+      </c>
+      <c r="F21" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="G21" s="47">
+      <c r="G21" s="63">
         <v>1</v>
       </c>
-      <c r="H21" s="47">
+      <c r="H21" s="63">
         <v>1</v>
       </c>
-      <c r="I21" s="48">
+      <c r="I21" s="47">
         <v>1</v>
       </c>
     </row>
@@ -5215,30 +5227,30 @@
       </c>
       <c r="B22" s="45">
         <f>MeOH_original_data!B19*1000/(24)</f>
-        <v>14666.666666666666</v>
+        <v>14458.333333333334</v>
       </c>
       <c r="C22" s="45">
         <f>MeOH_original_data!C19*1000/(24)</f>
-        <v>73375</v>
+        <v>72291.666666666672</v>
       </c>
       <c r="D22" s="46">
         <f>MeOH_original_data!D19*1000/(24)</f>
-        <v>146791.66666666666</v>
-      </c>
-      <c r="F22" s="52" t="s">
+        <v>144583.33333333334</v>
+      </c>
+      <c r="F22" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="G22" s="47">
+      <c r="G22" s="63">
         <f>G$21*B22/B$21</f>
-        <v>6.068965517241379</v>
-      </c>
-      <c r="H22" s="47">
+        <v>5.8813559322033901</v>
+      </c>
+      <c r="H22" s="63">
         <f t="shared" ref="H22:I23" si="1">H$21*C22/C21</f>
-        <v>6.0515463917525771</v>
-      </c>
-      <c r="I22" s="48">
+        <v>5.9215017064846416</v>
+      </c>
+      <c r="I22" s="47">
         <f>I$21*D22/D21</f>
-        <v>6.0428816466552311</v>
+        <v>5.9316239316239319</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5257,43 +5269,43 @@
         <f>MeOH_original_data!D20</f>
         <v>53</v>
       </c>
-      <c r="F23" s="52" t="s">
+      <c r="F23" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="G23" s="47">
+      <c r="G23" s="63">
         <f t="shared" ref="G23" si="2">G$21*B23/B$21</f>
-        <v>2.2758620689655173E-3</v>
-      </c>
-      <c r="H23" s="47">
+        <v>2.2372881355932203E-3</v>
+      </c>
+      <c r="H23" s="63">
         <f t="shared" si="1"/>
-        <v>3.6797274275979556E-4</v>
-      </c>
-      <c r="I23" s="48">
+        <v>3.7348703170028816E-4</v>
+      </c>
+      <c r="I23" s="47">
         <f t="shared" si="1"/>
-        <v>3.6105591825149024E-4</v>
+        <v>3.6657060518731984E-4</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="59"/>
-      <c r="F24" s="52" t="s">
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="57"/>
+      <c r="F24" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="47">
+      <c r="G24" s="63">
         <f>G$21*B25/B$21</f>
-        <v>4.1379310344827586E-2</v>
-      </c>
-      <c r="H24" s="47">
+        <v>1.4462431033898306</v>
+      </c>
+      <c r="H24" s="63">
         <f t="shared" ref="H24:I24" si="3">H$21*C25/C$21</f>
-        <v>4.192439862542955E-2</v>
-      </c>
-      <c r="I24" s="48">
+        <v>1.4552794228668944</v>
+      </c>
+      <c r="I24" s="47">
         <f t="shared" si="3"/>
-        <v>4.1852487135506003E-2</v>
+        <v>9.2287580000000008E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -5302,30 +5314,30 @@
       </c>
       <c r="B25" s="42">
         <f>MeOH_original_data!B22*1000/(24)</f>
-        <v>100</v>
+        <v>3555.347629166667</v>
       </c>
       <c r="C25" s="42">
         <f>MeOH_original_data!C22*1000/(24)</f>
-        <v>508.33333333333331</v>
+        <v>17766.536287500003</v>
       </c>
       <c r="D25" s="43">
         <f>MeOH_original_data!D22*1000/(24)</f>
-        <v>1016.6666666666666</v>
-      </c>
-      <c r="F25" s="52" t="s">
+        <v>2249.5097625000003</v>
+      </c>
+      <c r="F25" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="G25" s="47">
+      <c r="G25" s="63">
         <f t="shared" ref="G25:G26" si="4">G$21*B26/B$21</f>
-        <v>0.34655172413793106</v>
-      </c>
-      <c r="H25" s="47">
+        <v>0.40960135593220343</v>
+      </c>
+      <c r="H25" s="63">
         <f t="shared" ref="H25:H26" si="5">H$21*C26/C$21</f>
-        <v>0.3446735395189004</v>
-      </c>
-      <c r="I25" s="48">
+        <v>0.41283137201365194</v>
+      </c>
+      <c r="I25" s="47">
         <f t="shared" ref="I25:I26" si="6">I$21*D26/D$21</f>
-        <v>0.34425385934819897</v>
+        <v>0.41353706666666673</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5334,30 +5346,30 @@
       </c>
       <c r="B26" s="44">
         <f>MeOH_original_data!B23*1000/(24)</f>
-        <v>837.5</v>
+        <v>1006.9366666666668</v>
       </c>
       <c r="C26" s="44">
         <f>MeOH_original_data!C23*1000/(24)</f>
-        <v>4179.166666666667</v>
+        <v>5039.9830000000011</v>
       </c>
       <c r="D26" s="27">
         <f>MeOH_original_data!D23*1000/(24)</f>
-        <v>8362.5</v>
-      </c>
-      <c r="F26" s="53" t="s">
+        <v>10079.966000000002</v>
+      </c>
+      <c r="F26" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="G26" s="49">
+      <c r="G26" s="64">
         <f t="shared" si="4"/>
-        <v>1.4896551724137932</v>
-      </c>
-      <c r="H26" s="49">
+        <v>0.10078349152542374</v>
+      </c>
+      <c r="H26" s="64">
         <f t="shared" si="5"/>
-        <v>1.4838487972508592</v>
-      </c>
-      <c r="I26" s="50">
+        <v>0.10193266723549486</v>
+      </c>
+      <c r="I26" s="48">
         <f t="shared" si="6"/>
-        <v>1.481303602058319</v>
+        <v>1.6096854222222223</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5366,15 +5378,15 @@
       </c>
       <c r="B27" s="45">
         <f>MeOH_original_data!B24*1000/(24)</f>
-        <v>3600</v>
+        <v>247.75941666666668</v>
       </c>
       <c r="C27" s="45">
         <f>MeOH_original_data!C24*1000/(24)</f>
-        <v>17991.666666666668</v>
+        <v>1244.4279791666665</v>
       </c>
       <c r="D27" s="46">
         <f>MeOH_original_data!D24*1000/(24)</f>
-        <v>35983.333333333336</v>
+        <v>39236.082166666667</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -5520,15 +5532,15 @@
       </c>
       <c r="B43">
         <f>B21/B42</f>
-        <v>24.166666666666664</v>
+        <v>24.583333333333336</v>
       </c>
       <c r="C43">
         <f>C21/C42</f>
-        <v>24.25</v>
+        <v>24.416666666666668</v>
       </c>
       <c r="D43">
         <f>D21/D42</f>
-        <v>24.291666666666668</v>
+        <v>24.375</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -5537,7 +5549,7 @@
       </c>
       <c r="B44">
         <f>B43</f>
-        <v>24.166666666666664</v>
+        <v>24.583333333333336</v>
       </c>
     </row>
   </sheetData>
@@ -5552,10 +5564,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDBD3A5-912B-984E-9A90-BB156C754950}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5734,13 +5746,13 @@
         <v>144</v>
       </c>
       <c r="B18">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D18">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -5748,13 +5760,13 @@
         <v>155</v>
       </c>
       <c r="B19">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C19">
-        <v>1761</v>
+        <v>1735</v>
       </c>
       <c r="D19">
-        <v>3523</v>
+        <v>3470</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -5780,46 +5792,138 @@
       <c r="A22" t="s">
         <v>154</v>
       </c>
-      <c r="B22">
-        <v>2.4</v>
-      </c>
-      <c r="C22">
-        <v>12.2</v>
-      </c>
-      <c r="D22">
-        <v>24.4</v>
+      <c r="B22" s="39">
+        <f>B28*$B$32*$B34/1000</f>
+        <v>85.328343100000012</v>
+      </c>
+      <c r="C22" s="39">
+        <f t="shared" ref="C22:D22" si="0">C28*$B$32*$B34/1000</f>
+        <v>426.39687090000001</v>
+      </c>
+      <c r="D22" s="39">
+        <f t="shared" si="0"/>
+        <v>53.988234300000009</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>156</v>
       </c>
-      <c r="B23">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="C23">
-        <v>100.3</v>
-      </c>
-      <c r="D23">
-        <v>200.7</v>
+      <c r="B23" s="39">
+        <f t="shared" ref="B23:D23" si="1">B29*$B$32*$B35/1000</f>
+        <v>24.166480000000004</v>
+      </c>
+      <c r="C23" s="39">
+        <f t="shared" si="1"/>
+        <v>120.95959200000001</v>
+      </c>
+      <c r="D23" s="39">
+        <f>D29*$B$32*$B35/1000</f>
+        <v>241.91918400000003</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>157</v>
       </c>
-      <c r="B24">
-        <v>86.4</v>
-      </c>
-      <c r="C24">
-        <v>431.8</v>
-      </c>
-      <c r="D24">
-        <v>863.6</v>
+      <c r="B24" s="39">
+        <f t="shared" ref="B24:D24" si="2">B30*$B$32*$B36/1000</f>
+        <v>5.9462260000000002</v>
+      </c>
+      <c r="C24" s="39">
+        <f t="shared" si="2"/>
+        <v>29.8662715</v>
+      </c>
+      <c r="D24" s="39">
+        <f t="shared" si="2"/>
+        <v>941.66597200000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28">
+        <v>697</v>
+      </c>
+      <c r="C28">
+        <v>3483</v>
+      </c>
+      <c r="D28">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29">
+        <v>190</v>
+      </c>
+      <c r="C29">
+        <v>951</v>
+      </c>
+      <c r="D29">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30">
+        <v>44</v>
+      </c>
+      <c r="C30">
+        <v>221</v>
+      </c>
+      <c r="D30">
+        <v>6968</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>195</v>
+      </c>
+      <c r="B32">
+        <v>158.99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>157</v>
+      </c>
+      <c r="B36">
+        <v>0.85</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="E5wXOZaLLrrq7SCc6l+P2ZRx9IPEuRyCimf3Z0baz1pnEGajuwEnyXDqCBaOzjtZXMtVpsqDvw4pp6yfyAXdcg==" saltValue="DJDNe6oto2IcuT0txsQDEg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>